<commit_message>
Implement: add records to the data base (addresses #241)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\switch\projectg2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{028D1B2C-72FB-40A1-B769-FBE56F369CAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853F797-0B61-4BEA-8B24-7DD99A8002F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="6" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -5629,7 +5629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FF6538-20DF-4E13-8107-7AC155FD4D73}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -5970,8 +5970,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC3EF37-2BA8-4EC6-92A1-22C0C9AA6791}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7347,12 +7347,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b40f5c691649a4a05e2eddbeb14bcbeb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6aca1daf-af28-46f8-bd7f-7c486cf57d75" xmlns:ns3="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1826bf959a736503351b94de29104941" ns2:_="" ns3:_="">
     <xsd:import namespace="6aca1daf-af28-46f8-bd7f-7c486cf57d75"/>
@@ -7555,6 +7549,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7565,15 +7565,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6920F70-FC70-4BF2-86B7-0FEAC01D1483}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7592,6 +7583,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Implement: add records to the database (addresses #241)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\switch\projectg2\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Desktop\Projeto\projectg2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E853F797-0B61-4BEA-8B24-7DD99A8002F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C36AEF6-1AD0-41A7-A5BD-BF76C199944C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="8" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="938" activeTab="8" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,11 @@
   <externalReferences>
     <externalReference r:id="rId13"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">BacklogUSStatus!$A$1:$E$100</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ProjectBacklog!$A$1:$H$67</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +41,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -47,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1141" uniqueCount="403">
   <si>
     <t>id</t>
   </si>
@@ -950,6 +956,312 @@
   </si>
   <si>
     <t>TimeEstimate</t>
+  </si>
+  <si>
+    <t>2021-03-01</t>
+  </si>
+  <si>
+    <t>2021-06-01</t>
+  </si>
+  <si>
+    <t>2022-03-01</t>
+  </si>
+  <si>
+    <t>2021-07-31</t>
+  </si>
+  <si>
+    <t>2022-04-29</t>
+  </si>
+  <si>
+    <t>2021-06-20</t>
+  </si>
+  <si>
+    <t>2021-03-02</t>
+  </si>
+  <si>
+    <t>2021-03-03</t>
+  </si>
+  <si>
+    <t>2021-03-04</t>
+  </si>
+  <si>
+    <t>2021-03-05</t>
+  </si>
+  <si>
+    <t>2021-03-07</t>
+  </si>
+  <si>
+    <t>2021-03-08</t>
+  </si>
+  <si>
+    <t>2021-03-10</t>
+  </si>
+  <si>
+    <t>2021-03-22</t>
+  </si>
+  <si>
+    <t>2021-04-05</t>
+  </si>
+  <si>
+    <t>2021-04-26</t>
+  </si>
+  <si>
+    <t>2021-05-10</t>
+  </si>
+  <si>
+    <t>2021-05-24</t>
+  </si>
+  <si>
+    <t>2021-06-07</t>
+  </si>
+  <si>
+    <t>2021-06-21</t>
+  </si>
+  <si>
+    <t>2021-07-19</t>
+  </si>
+  <si>
+    <t>2021-07-05</t>
+  </si>
+  <si>
+    <t>2021-08-02</t>
+  </si>
+  <si>
+    <t>2021-08-30</t>
+  </si>
+  <si>
+    <t>2021-09-27</t>
+  </si>
+  <si>
+    <t>2021-10-18</t>
+  </si>
+  <si>
+    <t>2021-11-15</t>
+  </si>
+  <si>
+    <t>2021-12-06</t>
+  </si>
+  <si>
+    <t>2022-01-10</t>
+  </si>
+  <si>
+    <t>2022-02-07</t>
+  </si>
+  <si>
+    <t>2022-03-07</t>
+  </si>
+  <si>
+    <t>2022-04-04</t>
+  </si>
+  <si>
+    <t>2021-06-02</t>
+  </si>
+  <si>
+    <t>2021-06-04</t>
+  </si>
+  <si>
+    <t>us_start</t>
+  </si>
+  <si>
+    <t>US_ID</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US01</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US02</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US03</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US04</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US05</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US06</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US07</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US08</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US09</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US10</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US11</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US12</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US13</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US14</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US15</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US16</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US17</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US18</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US19</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US20</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US21</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US22</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US23</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US24</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US25</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US26</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US27</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US28</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US29</t>
+  </si>
+  <si>
+    <t>Project_2022_1&amp;as want US30</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US001</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US002</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US003</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US004</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US005</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US006</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US007</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US008</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US009</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US010</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US011</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US012</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US013</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US014</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US015</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US016</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US017</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US018</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US019</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US020</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US021</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US022</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US023</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US024</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US025</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US026</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US027</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US028</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US029</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US030</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US031</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US032</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US033</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US034</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US035</t>
+  </si>
+  <si>
+    <t>Project_2022_2&amp;as want US036</t>
   </si>
 </sst>
 </file>
@@ -959,7 +1271,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1010,6 +1322,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1050,7 +1369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1068,16 +1387,22 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1240,7 +1565,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2072,8 +2397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E62CEF3-4F99-4CE5-B31F-511FA523F4D9}">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3706,6 +4031,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:E100" xr:uid="{9E62CEF3-4F99-4CE5-B31F-511FA523F4D9}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B94:B97">
     <sortCondition ref="B94:B97"/>
   </sortState>
@@ -4865,10 +5191,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59AF7EF-B12B-4A6F-9425-B1B26B554B1A}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G1" sqref="G1:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4885,10 +5211,10 @@
     <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>56</v>
       </c>
@@ -4907,10 +5233,10 @@
       <c r="F1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="20" t="s">
         <v>212</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="21" t="s">
         <v>213</v>
       </c>
       <c r="I1" s="1" t="s">
@@ -4925,11 +5251,11 @@
       <c r="L1" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>218</v>
       </c>
@@ -4948,11 +5274,11 @@
       <c r="F2" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="17">
-        <v>44256</v>
-      </c>
-      <c r="H2" s="17">
-        <v>44408</v>
+      <c r="G2" s="10" t="s">
+        <v>301</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>304</v>
       </c>
       <c r="I2" t="str">
         <f>TEXT(8,"0")</f>
@@ -4974,12 +5300,11 @@
       <c r="O2" s="10"/>
       <c r="P2" s="10"/>
       <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10" t="s">
+      <c r="R2" s="10" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>219</v>
       </c>
@@ -4998,11 +5323,11 @@
       <c r="F3" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="17">
-        <v>44348</v>
-      </c>
-      <c r="H3" s="17">
-        <v>44680</v>
+      <c r="G3" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>305</v>
       </c>
       <c r="I3" t="str">
         <f>TEXT(12,"0")</f>
@@ -5024,12 +5349,11 @@
       <c r="O3" s="10"/>
       <c r="P3" s="10"/>
       <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10" t="s">
+      <c r="R3" s="10" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>220</v>
       </c>
@@ -5048,10 +5372,10 @@
       <c r="F4" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="17">
-        <v>44630</v>
-      </c>
-      <c r="H4" s="17"/>
+      <c r="G4" s="10" t="s">
+        <v>303</v>
+      </c>
+      <c r="H4" s="15"/>
       <c r="I4" t="str">
         <f>TEXT(15,"0")</f>
         <v>15</v>
@@ -5073,9 +5397,8 @@
       <c r="P4" s="10"/>
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -5094,13 +5417,12 @@
       <c r="P5" s="10"/>
       <c r="Q5" s="10"/>
       <c r="R5" s="10"/>
-      <c r="S5" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F4 E7:F14 G7:G8" xr:uid="{67CE1979-44A6-4EF0-9F88-D467BDB4AAA6}">
-      <formula1>$S$2:$S$3</formula1>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:F4 G7:G8 E7:F14" xr:uid="{67CE1979-44A6-4EF0-9F88-D467BDB4AAA6}">
+      <formula1>$R$2:$R$3</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5297,7 +5619,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5308,16 +5630,16 @@
     <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="4"/>
-    <col min="9" max="9" width="9.21875" style="4"/>
-    <col min="10" max="10" width="14.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="7"/>
+    <col min="9" max="9" width="9.21875" style="7"/>
+    <col min="10" max="10" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>221</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="20" t="s">
         <v>222</v>
       </c>
       <c r="C1" s="8" t="s">
@@ -5329,24 +5651,24 @@
       <c r="E1" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="16" t="s">
         <v>224</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="16" t="s">
         <v>225</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="I1" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="8" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="13" t="s">
         <v>198</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -5355,31 +5677,31 @@
       <c r="C2" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="D2" s="2">
-        <v>44198</v>
-      </c>
-      <c r="E2" s="2">
-        <v>44408</v>
-      </c>
-      <c r="F2" s="19">
+      <c r="D2" s="10" t="s">
+        <v>307</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="F2" s="17">
         <v>35</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="17">
         <v>0.2</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="7">
         <v>1237</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="7">
         <v>4</v>
       </c>
-      <c r="J2" s="4" t="str">
+      <c r="J2" s="7" t="str">
         <f>VLOOKUP(H2,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Tiago Cancado</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="13" t="s">
         <v>195</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -5388,31 +5710,31 @@
       <c r="C3" s="7" t="s">
         <v>228</v>
       </c>
-      <c r="D3" s="2">
-        <v>44199</v>
-      </c>
-      <c r="E3" s="2">
-        <v>44408</v>
-      </c>
-      <c r="F3" s="19">
+      <c r="D3" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="F3" s="17">
         <v>25</v>
       </c>
-      <c r="G3" s="19">
+      <c r="G3" s="17">
         <v>0.2</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="7">
         <v>1234</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="7">
         <v>5</v>
       </c>
-      <c r="J3" s="4" t="str">
+      <c r="J3" s="7" t="str">
         <f>VLOOKUP(H3,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Joao Silva</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>196</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -5421,31 +5743,31 @@
       <c r="C4" s="7" t="s">
         <v>227</v>
       </c>
-      <c r="D4" s="2">
-        <v>44200</v>
-      </c>
-      <c r="E4" s="2">
-        <v>44408</v>
-      </c>
-      <c r="F4" s="19">
+      <c r="D4" s="10" t="s">
+        <v>309</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="F4" s="17">
         <v>25</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="17">
         <v>0.3</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="7">
         <v>1235</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="7">
         <v>6</v>
       </c>
-      <c r="J4" s="4" t="str">
+      <c r="J4" s="7" t="str">
         <f>VLOOKUP(H4,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Manel Costa</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="A5" s="13" t="s">
         <v>197</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -5454,31 +5776,31 @@
       <c r="C5" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="D5" s="2">
-        <v>44201</v>
-      </c>
-      <c r="E5" s="2">
-        <v>44408</v>
-      </c>
-      <c r="F5" s="19">
+      <c r="D5" s="10" t="s">
+        <v>310</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="F5" s="17">
         <v>20</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="17">
         <v>1</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="7">
         <v>1236</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="7">
         <v>7</v>
       </c>
-      <c r="J5" s="4" t="str">
+      <c r="J5" s="7" t="str">
         <f>VLOOKUP(H5,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Xico Ferreira</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -5487,31 +5809,31 @@
       <c r="C6" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="D6" s="2">
-        <v>44203</v>
-      </c>
-      <c r="E6" s="2">
-        <v>44408</v>
-      </c>
-      <c r="F6" s="19">
+      <c r="D6" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>304</v>
+      </c>
+      <c r="F6" s="17">
         <v>20</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="17">
         <v>1</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="7">
         <v>1241</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="7">
         <v>7</v>
       </c>
-      <c r="J6" s="4" t="str">
+      <c r="J6" s="7" t="str">
         <f>VLOOKUP(H6,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Nel Moleiro</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="13" t="s">
         <v>200</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -5520,31 +5842,31 @@
       <c r="C7" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="D7" s="2">
-        <v>44204</v>
-      </c>
-      <c r="E7" s="2">
-        <v>44367</v>
-      </c>
-      <c r="F7" s="19">
+      <c r="D7" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F7" s="17">
         <v>20</v>
       </c>
-      <c r="G7" s="19">
+      <c r="G7" s="17">
         <v>1</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="7">
         <v>1243</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="7">
         <v>7</v>
       </c>
-      <c r="J7" s="4" t="str">
+      <c r="J7" s="7" t="str">
         <f>VLOOKUP(H7,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Zé do Bento</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="13" t="s">
         <v>36</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -5553,31 +5875,31 @@
       <c r="C8" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="D8" s="2">
-        <v>44204</v>
-      </c>
-      <c r="E8" s="2">
-        <v>44367</v>
-      </c>
-      <c r="F8" s="19">
+      <c r="D8" s="10" t="s">
+        <v>312</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F8" s="17">
         <v>20</v>
       </c>
-      <c r="G8" s="19">
+      <c r="G8" s="17">
         <v>1</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="7">
         <v>1246</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="7">
         <v>7</v>
       </c>
-      <c r="J8" s="4" t="str">
+      <c r="J8" s="7" t="str">
         <f>VLOOKUP(H8,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Tó Farrulo</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="13" t="s">
         <v>38</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -5586,51 +5908,42 @@
       <c r="C9" s="7" t="s">
         <v>226</v>
       </c>
-      <c r="D9" s="2">
-        <v>44206</v>
-      </c>
-      <c r="E9" s="2">
-        <v>44367</v>
-      </c>
-      <c r="F9" s="19">
+      <c r="D9" s="10" t="s">
+        <v>313</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>306</v>
+      </c>
+      <c r="F9" s="17">
         <v>20</v>
       </c>
-      <c r="G9" s="19">
+      <c r="G9" s="17">
         <v>1</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="7">
         <v>1247</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="7">
         <v>7</v>
       </c>
-      <c r="J9" s="4" t="str">
+      <c r="J9" s="7" t="str">
         <f>VLOOKUP(H9,[1]Users!$A$2:$B$50,2,FALSE)</f>
         <v>Tino das Cruzes</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{EAEAD8CA-C370-41C4-8B48-57731DCEA4EA}"/>
-    <hyperlink ref="A3" r:id="rId2" xr:uid="{BE0FCCDD-8613-404C-9DD1-C53415F77BCE}"/>
-    <hyperlink ref="A4" r:id="rId3" xr:uid="{14D5B301-F4AE-4489-9321-75066BF13FFD}"/>
-    <hyperlink ref="A5" r:id="rId4" xr:uid="{2CFB36F5-19BC-4729-A122-7B8BAC2C5B9E}"/>
-    <hyperlink ref="A7" r:id="rId5" xr:uid="{ED1F0B00-34ED-4229-A42F-D06D06B0EC53}"/>
-    <hyperlink ref="A6" r:id="rId6" xr:uid="{ED1B573C-BDB0-472B-8F8F-A9F4A7241CB7}"/>
-    <hyperlink ref="A8" r:id="rId7" xr:uid="{B44C5183-07F7-47B9-AAB0-EEBD30DDEE28}"/>
-    <hyperlink ref="A9" r:id="rId8" xr:uid="{9445C0C4-334E-4BC3-BC96-FCAF1B2C5CE9}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FF6538-20DF-4E13-8107-7AC155FD4D73}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5641,7 +5954,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="20" t="s">
         <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -5659,8 +5972,8 @@
         <f>TEXT(1,"0")</f>
         <v>1</v>
       </c>
-      <c r="C2" s="2">
-        <v>44277</v>
+      <c r="C2" s="10" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -5671,8 +5984,8 @@
         <f>TEXT(2,"0")</f>
         <v>2</v>
       </c>
-      <c r="C3" s="2">
-        <v>44291</v>
+      <c r="C3" s="10" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -5683,8 +5996,8 @@
         <f>TEXT(3,"0")</f>
         <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>44312</v>
+      <c r="C4" s="10" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -5695,8 +6008,8 @@
         <f>TEXT(4,"0")</f>
         <v>4</v>
       </c>
-      <c r="C5" s="2">
-        <v>44326</v>
+      <c r="C5" s="10" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -5707,8 +6020,8 @@
         <f>TEXT(5,"0")</f>
         <v>5</v>
       </c>
-      <c r="C6" s="2">
-        <v>44340</v>
+      <c r="C6" s="10" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -5719,8 +6032,8 @@
         <f>TEXT(6,"0")</f>
         <v>6</v>
       </c>
-      <c r="C7" s="2">
-        <v>44354</v>
+      <c r="C7" s="10" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -5731,8 +6044,8 @@
         <f>TEXT(7,"0")</f>
         <v>7</v>
       </c>
-      <c r="C8" s="2">
-        <v>44368</v>
+      <c r="C8" s="10" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -5743,8 +6056,8 @@
         <f>TEXT(8,"0")</f>
         <v>8</v>
       </c>
-      <c r="C9" s="2">
-        <v>44396</v>
+      <c r="C9" s="10" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -5755,8 +6068,8 @@
         <f>TEXT(1,"0")</f>
         <v>1</v>
       </c>
-      <c r="C10" s="2">
-        <v>44354</v>
+      <c r="C10" s="10" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -5767,8 +6080,8 @@
         <f>TEXT(2,"0")</f>
         <v>2</v>
       </c>
-      <c r="C11" s="2">
-        <v>44382</v>
+      <c r="C11" s="10" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -5779,8 +6092,8 @@
         <f>TEXT(3,"0")</f>
         <v>3</v>
       </c>
-      <c r="C12" s="2">
-        <v>44410</v>
+      <c r="C12" s="10" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -5791,8 +6104,8 @@
         <f>TEXT(4,"0")</f>
         <v>4</v>
       </c>
-      <c r="C13" s="2">
-        <v>44438</v>
+      <c r="C13" s="10" t="s">
+        <v>324</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -5803,8 +6116,8 @@
         <f>TEXT(5,"0")</f>
         <v>5</v>
       </c>
-      <c r="C14" s="2">
-        <v>44466</v>
+      <c r="C14" s="10" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -5815,8 +6128,8 @@
         <f>TEXT(6,"0")</f>
         <v>6</v>
       </c>
-      <c r="C15" s="2">
-        <v>44487</v>
+      <c r="C15" s="10" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -5827,8 +6140,8 @@
         <f>TEXT(7,"0")</f>
         <v>7</v>
       </c>
-      <c r="C16" s="2">
-        <v>44515</v>
+      <c r="C16" s="10" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -5839,8 +6152,8 @@
         <f>TEXT(8,"0")</f>
         <v>8</v>
       </c>
-      <c r="C17" s="2">
-        <v>44536</v>
+      <c r="C17" s="10" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -5851,8 +6164,8 @@
         <f>TEXT(9,"0")</f>
         <v>9</v>
       </c>
-      <c r="C18" s="2">
-        <v>44571</v>
+      <c r="C18" s="10" t="s">
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -5863,8 +6176,8 @@
         <f>TEXT(10,"0")</f>
         <v>10</v>
       </c>
-      <c r="C19" s="2">
-        <v>44599</v>
+      <c r="C19" s="10" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -5875,8 +6188,8 @@
         <f>TEXT(11,"0")</f>
         <v>11</v>
       </c>
-      <c r="C20" s="2">
-        <v>44627</v>
+      <c r="C20" s="10" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -5887,12 +6200,9 @@
         <f>TEXT(12,"0")</f>
         <v>12</v>
       </c>
-      <c r="C21" s="2">
-        <v>44655</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C22" s="2"/>
+      <c r="C21" s="10" t="s">
+        <v>332</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5970,37 +6280,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC3EF37-2BA8-4EC6-92A1-22C0C9AA6791}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H42" sqref="H42:H66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.44140625" style="25" customWidth="1"/>
     <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="18"/>
+    <col min="4" max="4" width="15.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="24" t="s">
         <v>230</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="23" t="s">
         <v>167</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="21" t="s">
         <v>86</v>
+      </c>
+      <c r="G1" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>335</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>10</v>
@@ -6010,20 +6328,26 @@
       <c r="A2" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="20">
+      <c r="C2" s="18">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="21">
+      <c r="E2" s="19">
         <v>10</v>
       </c>
-      <c r="F2" t="s">
-        <v>87</v>
+      <c r="F2" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="25" t="s">
+        <v>337</v>
+      </c>
+      <c r="H2" s="26" t="s">
+        <v>307</v>
       </c>
       <c r="O2" t="s">
         <v>88</v>
@@ -6033,21 +6357,25 @@
       <c r="A3" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="C3" s="20">
+      <c r="C3" s="18">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E3" s="21">
+      <c r="E3" s="19">
         <v>15</v>
       </c>
-      <c r="F3" t="s">
-        <v>87</v>
-      </c>
+      <c r="F3" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>338</v>
+      </c>
+      <c r="H3" s="13"/>
       <c r="O3" t="s">
         <v>87</v>
       </c>
@@ -6056,21 +6384,25 @@
       <c r="A4" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>235</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="18">
         <v>3</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="19">
         <v>11</v>
       </c>
-      <c r="F4" t="s">
-        <v>87</v>
-      </c>
+      <c r="F4" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G4" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="H4" s="13"/>
       <c r="O4" t="s">
         <v>90</v>
       </c>
@@ -6079,1260 +6411,1518 @@
       <c r="A5" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="C5" s="20">
+      <c r="C5" s="18">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
-        <v>87</v>
-      </c>
+      <c r="F5" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>340</v>
+      </c>
+      <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="C6" s="20">
+      <c r="C6" s="18">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>13.5</v>
       </c>
-      <c r="F6" t="s">
-        <v>87</v>
-      </c>
+      <c r="F6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>341</v>
+      </c>
+      <c r="H6" s="13"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>238</v>
       </c>
-      <c r="C7" s="20">
+      <c r="C7" s="18">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="19">
         <v>14</v>
       </c>
-      <c r="F7" t="s">
-        <v>87</v>
-      </c>
+      <c r="F7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>342</v>
+      </c>
+      <c r="H7" s="13"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="10" t="s">
         <v>239</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="18">
         <v>2</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="19">
         <v>14.5</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="10" t="s">
         <v>88</v>
+      </c>
+      <c r="G8" s="25" t="s">
+        <v>343</v>
+      </c>
+      <c r="H8" s="26" t="s">
+        <v>307</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="10" t="s">
         <v>240</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="18">
         <v>3</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="19">
         <v>15</v>
       </c>
-      <c r="F9" t="s">
-        <v>87</v>
-      </c>
+      <c r="F9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="18">
         <v>4</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="19">
         <v>15.5</v>
       </c>
-      <c r="F10" t="s">
-        <v>87</v>
-      </c>
+      <c r="F10" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>345</v>
+      </c>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="10" t="s">
         <v>242</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="18">
         <v>5</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="19">
         <v>16</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="10" t="s">
         <v>90</v>
       </c>
+      <c r="G11" s="25" t="s">
+        <v>346</v>
+      </c>
+      <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="10" t="s">
         <v>243</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="18">
         <v>1</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="19">
         <v>16.5</v>
       </c>
-      <c r="F12" t="s">
-        <v>87</v>
-      </c>
+      <c r="F12" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>347</v>
+      </c>
+      <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="18">
         <v>2</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="19">
         <v>17</v>
       </c>
-      <c r="F13" t="s">
-        <v>87</v>
-      </c>
+      <c r="F13" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G13" s="25" t="s">
+        <v>348</v>
+      </c>
+      <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="10" t="s">
         <v>245</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="18">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="19">
         <v>17.5</v>
       </c>
-      <c r="F14" t="s">
-        <v>87</v>
-      </c>
+      <c r="F14" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>349</v>
+      </c>
+      <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="10" t="s">
         <v>246</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="18">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="19">
         <v>18</v>
       </c>
-      <c r="F15" t="s">
-        <v>87</v>
-      </c>
+      <c r="F15" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="25" t="s">
+        <v>350</v>
+      </c>
+      <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="18">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="19">
         <v>18.5</v>
       </c>
-      <c r="F16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F16" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>351</v>
+      </c>
+      <c r="H16" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="10" t="s">
         <v>248</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="18">
         <v>1</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="19">
         <v>19</v>
       </c>
-      <c r="F17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F17" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G17" s="25" t="s">
+        <v>352</v>
+      </c>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="10" t="s">
         <v>249</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="18">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="19">
         <v>19.5</v>
       </c>
-      <c r="F18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F18" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G18" s="25" t="s">
+        <v>353</v>
+      </c>
+      <c r="H18" s="13"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="18">
         <v>3</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="19">
         <v>20</v>
       </c>
-      <c r="F19" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F19" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G19" s="25" t="s">
+        <v>354</v>
+      </c>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="10" t="s">
         <v>251</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="18">
         <v>4</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="19">
         <v>20.5</v>
       </c>
-      <c r="F20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F20" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>355</v>
+      </c>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="18">
         <v>5</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="19">
         <v>21</v>
       </c>
-      <c r="F21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F21" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G21" s="25" t="s">
+        <v>356</v>
+      </c>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="18">
         <v>1</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="19">
         <v>21.5</v>
       </c>
-      <c r="F22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F22" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G22" s="25" t="s">
+        <v>357</v>
+      </c>
+      <c r="H22" s="13"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="18">
         <v>2</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="19">
         <v>22</v>
       </c>
-      <c r="F23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G23" s="25" t="s">
+        <v>358</v>
+      </c>
+      <c r="H23" s="13"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="10" t="s">
         <v>255</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="18">
         <v>3</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="E24" s="21">
+      <c r="E24" s="19">
         <v>22.5</v>
       </c>
-      <c r="F24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F24" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>359</v>
+      </c>
+      <c r="H24" s="13"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="10" t="s">
         <v>256</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="18">
         <v>4</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="E25" s="21">
+      <c r="E25" s="19">
         <v>23</v>
       </c>
-      <c r="F25" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F25" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>360</v>
+      </c>
+      <c r="H25" s="13"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="10" t="s">
         <v>257</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="18">
         <v>5</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="19">
         <v>23.5</v>
       </c>
-      <c r="F26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F26" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>361</v>
+      </c>
+      <c r="H26" s="13"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="18">
         <v>1</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D27" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="19">
         <v>24</v>
       </c>
-      <c r="F27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F27" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G27" s="25" t="s">
+        <v>362</v>
+      </c>
+      <c r="H27" s="13"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="18">
         <v>2</v>
       </c>
-      <c r="D28" t="s">
+      <c r="D28" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="19">
         <v>24.5</v>
       </c>
-      <c r="F28" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F28" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" s="25" t="s">
+        <v>363</v>
+      </c>
+      <c r="H28" s="13"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="18">
         <v>3</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D29" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="21">
+      <c r="E29" s="19">
         <v>25</v>
       </c>
-      <c r="F29" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F29" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" s="25" t="s">
+        <v>364</v>
+      </c>
+      <c r="H29" s="13"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="18">
         <v>4</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E30" s="21">
+      <c r="E30" s="19">
         <v>25.5</v>
       </c>
-      <c r="F30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F30" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="25" t="s">
+        <v>365</v>
+      </c>
+      <c r="H30" s="13"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="18">
         <v>5</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D31" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="19">
         <v>26</v>
       </c>
-      <c r="F31" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="10" t="s">
+      <c r="F31" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" s="25" t="s">
+        <v>366</v>
+      </c>
+      <c r="H31" s="13"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="18">
         <v>1</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D32" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="E32" s="21">
+      <c r="E32" s="19">
         <v>26.5</v>
       </c>
-      <c r="F32" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F32" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="H32" s="13"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B33" s="10" t="s">
         <v>264</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="18">
         <v>2</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="10" t="s">
         <v>131</v>
       </c>
-      <c r="E33" s="21">
+      <c r="E33" s="19">
         <v>27</v>
       </c>
-      <c r="F33" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F33" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G33" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="H33" s="13"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="10" t="s">
         <v>265</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="18">
         <v>3</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D34" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="E34" s="21">
+      <c r="E34" s="19">
         <v>27.5</v>
       </c>
-      <c r="F34" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F34" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G34" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="H34" s="13"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="10" t="s">
         <v>266</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="18">
         <v>4</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="E35" s="21">
+      <c r="E35" s="19">
         <v>28</v>
       </c>
-      <c r="F35" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F35" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G35" s="25" t="s">
+        <v>370</v>
+      </c>
+      <c r="H35" s="13"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B36" s="10" t="s">
         <v>267</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="18">
         <v>5</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D36" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="E36" s="21">
+      <c r="E36" s="19">
         <v>28.5</v>
       </c>
-      <c r="F36" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F36" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G36" s="25" t="s">
+        <v>371</v>
+      </c>
+      <c r="H36" s="13"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B37" s="10" t="s">
         <v>268</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="18">
         <v>1</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D37" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="E37" s="21">
+      <c r="E37" s="19">
         <v>29</v>
       </c>
-      <c r="F37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F37" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" s="25" t="s">
+        <v>372</v>
+      </c>
+      <c r="H37" s="13"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B38" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="18">
         <v>2</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="E38" s="21">
+      <c r="E38" s="19">
         <v>29.5</v>
       </c>
-      <c r="F38" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F38" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38" s="25" t="s">
+        <v>373</v>
+      </c>
+      <c r="H38" s="13"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B39" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="18">
         <v>3</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D39" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E39" s="19">
         <v>30</v>
       </c>
-      <c r="F39" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F39" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" s="25" t="s">
+        <v>374</v>
+      </c>
+      <c r="H39" s="13"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B40" s="10" t="s">
         <v>271</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="18">
         <v>4</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D40" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E40" s="21">
+      <c r="E40" s="19">
         <v>30.5</v>
       </c>
-      <c r="F40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F40" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G40" s="25" t="s">
+        <v>375</v>
+      </c>
+      <c r="H40" s="13"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B41" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="18">
         <v>5</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D41" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="21">
+      <c r="E41" s="19">
         <v>31</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F41" s="10" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G41" s="25" t="s">
+        <v>376</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="C42" s="20">
+      <c r="C42" s="18">
         <v>1</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="19">
         <v>31.5</v>
       </c>
-      <c r="F42" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F42" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G42" s="25" t="s">
+        <v>377</v>
+      </c>
+      <c r="H42" s="13"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="C43" s="20">
+      <c r="C43" s="18">
         <v>2</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="E43" s="21">
+      <c r="E43" s="19">
         <v>32</v>
       </c>
-      <c r="F43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F43" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G43" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="H43" s="13"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="18">
         <v>3</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E44" s="21">
+      <c r="E44" s="19">
         <v>32.5</v>
       </c>
-      <c r="F44" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F44" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G44" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="H44" s="13"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="C45" s="20">
+      <c r="C45" s="18">
         <v>4</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="E45" s="21">
+      <c r="E45" s="19">
         <v>33</v>
       </c>
-      <c r="F45" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F45" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G45" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="H45" s="13"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="C46" s="20">
+      <c r="C46" s="18">
         <v>5</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D46" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="E46" s="21">
+      <c r="E46" s="19">
         <v>33.5</v>
       </c>
-      <c r="F46" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F46" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="H46" s="13"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B47" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="18">
         <v>1</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D47" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="E47" s="21">
+      <c r="E47" s="19">
         <v>34</v>
       </c>
-      <c r="F47" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F47" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G47" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="H47" s="13"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="C48" s="20">
+      <c r="C48" s="18">
         <v>2</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E48" s="19">
         <v>34.5</v>
       </c>
-      <c r="F48" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F48" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G48" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="H48" s="13"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B49" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C49" s="18">
         <v>3</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D49" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="E49" s="21">
+      <c r="E49" s="19">
         <v>35</v>
       </c>
-      <c r="F49" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F49" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G49" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="H49" s="13"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B50" s="10" t="s">
         <v>281</v>
       </c>
-      <c r="C50" s="20">
+      <c r="C50" s="18">
         <v>4</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D50" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E50" s="21">
+      <c r="E50" s="19">
         <v>35.5</v>
       </c>
-      <c r="F50" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F50" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G50" s="25" t="s">
+        <v>385</v>
+      </c>
+      <c r="H50" s="13"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="10" t="s">
         <v>282</v>
       </c>
-      <c r="C51" s="20">
+      <c r="C51" s="18">
         <v>5</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="E51" s="21">
+      <c r="E51" s="19">
         <v>36</v>
       </c>
-      <c r="F51" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F51" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G51" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="H51" s="13"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B52" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="C52" s="20">
+      <c r="C52" s="18">
         <v>1</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="E52" s="21">
+      <c r="E52" s="19">
         <v>36.5</v>
       </c>
-      <c r="F52" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F52" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G52" s="25" t="s">
+        <v>387</v>
+      </c>
+      <c r="H52" s="13"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B53" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="C53" s="20">
+      <c r="C53" s="18">
         <v>2</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="E53" s="21">
+      <c r="E53" s="19">
         <v>37</v>
       </c>
-      <c r="F53" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F53" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G53" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="H53" s="13"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B54" t="s">
+      <c r="B54" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="C54" s="20">
+      <c r="C54" s="18">
         <v>3</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D54" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="E54" s="21">
+      <c r="E54" s="19">
         <v>37.5</v>
       </c>
-      <c r="F54" t="s">
+      <c r="F54" s="10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" s="25" t="s">
+        <v>389</v>
+      </c>
+      <c r="H54" s="13"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B55" t="s">
+      <c r="B55" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="C55" s="20">
+      <c r="C55" s="18">
         <v>4</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D55" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="E55" s="21">
+      <c r="E55" s="19">
         <v>38</v>
       </c>
-      <c r="F55" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F55" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G55" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="H55" s="13"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B56" s="10" t="s">
         <v>287</v>
       </c>
-      <c r="C56" s="20">
+      <c r="C56" s="18">
         <v>5</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D56" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="E56" s="21">
+      <c r="E56" s="19">
         <v>38.5</v>
       </c>
-      <c r="F56" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F56" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G56" s="25" t="s">
+        <v>391</v>
+      </c>
+      <c r="H56" s="13"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B57" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="C57" s="20">
+      <c r="C57" s="18">
         <v>1</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D57" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="21">
+      <c r="E57" s="19">
         <v>39</v>
       </c>
-      <c r="F57" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F57" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G57" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="H57" s="13"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B58" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="C58" s="20">
+      <c r="C58" s="18">
         <v>2</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D58" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="E58" s="21">
+      <c r="E58" s="19">
         <v>39.5</v>
       </c>
-      <c r="F58" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F58" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G58" s="25" t="s">
+        <v>393</v>
+      </c>
+      <c r="H58" s="13"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B59" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="C59" s="20">
+      <c r="C59" s="18">
         <v>3</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D59" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="E59" s="21">
+      <c r="E59" s="19">
         <v>40</v>
       </c>
-      <c r="F59" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F59" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G59" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="H59" s="13"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B60" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="C60" s="20">
+      <c r="C60" s="18">
         <v>4</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D60" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E60" s="21">
+      <c r="E60" s="19">
         <v>40.5</v>
       </c>
-      <c r="F60" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F60" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G60" s="25" t="s">
+        <v>395</v>
+      </c>
+      <c r="H60" s="13"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B61" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="C61" s="20">
+      <c r="C61" s="18">
         <v>5</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D61" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="E61" s="21">
+      <c r="E61" s="19">
         <v>41</v>
       </c>
-      <c r="F61" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F61" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G61" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="H61" s="13"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B62" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="C62" s="20">
+      <c r="C62" s="18">
         <v>1</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D62" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E62" s="21">
+      <c r="E62" s="19">
         <v>41.5</v>
       </c>
-      <c r="F62" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F62" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G62" s="25" t="s">
+        <v>397</v>
+      </c>
+      <c r="H62" s="13"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B63" t="s">
+      <c r="B63" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="C63" s="20">
+      <c r="C63" s="18">
         <v>2</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D63" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="E63" s="21">
+      <c r="E63" s="19">
         <v>42</v>
       </c>
-      <c r="F63" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F63" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G63" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="H63" s="13"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B64" t="s">
+      <c r="B64" s="10" t="s">
         <v>295</v>
       </c>
-      <c r="C64" s="20">
+      <c r="C64" s="18">
         <v>3</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D64" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="E64" s="21">
+      <c r="E64" s="19">
         <v>42.5</v>
       </c>
-      <c r="F64" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F64" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G64" s="25" t="s">
+        <v>399</v>
+      </c>
+      <c r="H64" s="13"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B65" t="s">
+      <c r="B65" s="10" t="s">
         <v>296</v>
       </c>
-      <c r="C65" s="20">
+      <c r="C65" s="18">
         <v>4</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D65" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E65" s="21">
+      <c r="E65" s="19">
         <v>43</v>
       </c>
-      <c r="F65" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F65" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G65" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="H65" s="13"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="10" t="s">
         <v>297</v>
       </c>
-      <c r="C66" s="20">
+      <c r="C66" s="18">
         <v>5</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="E66" s="21">
+      <c r="E66" s="19">
         <v>43.5</v>
       </c>
-      <c r="F66" t="s">
+      <c r="F66" s="10" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G66" s="25" t="s">
+        <v>401</v>
+      </c>
+      <c r="H66" s="13"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="C67" s="20">
+      <c r="C67" s="18">
         <v>1</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E67" s="21">
+      <c r="E67" s="19">
         <v>44</v>
       </c>
-      <c r="F67" t="s">
+      <c r="F67" s="10" t="s">
         <v>88</v>
+      </c>
+      <c r="G67" s="25" t="s">
+        <v>402</v>
+      </c>
+      <c r="H67" s="26" t="s">
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -7343,10 +7933,17 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005836243B3C47804EAF5FFDD9F066FCC7" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b40f5c691649a4a05e2eddbeb14bcbeb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6aca1daf-af28-46f8-bd7f-7c486cf57d75" xmlns:ns3="a1e3ca88-8ae5-4fd0-ba37-40ce669fcbb0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1826bf959a736503351b94de29104941" ns2:_="" ns3:_="">
     <xsd:import namespace="6aca1daf-af28-46f8-bd7f-7c486cf57d75"/>
@@ -7549,12 +8146,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -7565,6 +8156,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F6920F70-FC70-4BF2-86B7-0FEAC01D1483}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7583,15 +8183,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
US009 : Code Reengineering (addresses #191) Implement: add records to the database (addresses #241)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\switch\projectg2\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\crist\Desktop\Projeto\projectg2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9D68A96-D6C1-48A0-9A64-3BB600956808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F21B369-9F9A-4113-A1F9-FD092C491900}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8472" yWindow="1680" windowWidth="17280" windowHeight="8964" tabRatio="938" firstSheet="4" activeTab="8" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" tabRatio="938" activeTab="8" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,9 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">BacklogUSStatus!$A$1:$E$100</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ProjectBacklog!$A$1:$H$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ProjectBacklog!$A$1:$I$67</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -41,7 +41,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="400">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1158" uniqueCount="402">
   <si>
     <t>id</t>
   </si>
@@ -1251,6 +1253,12 @@
   </si>
   <si>
     <t>Project_2022_2&amp;as want US036</t>
+  </si>
+  <si>
+    <t>us_end</t>
+  </si>
+  <si>
+    <t>2021-04-02</t>
   </si>
 </sst>
 </file>
@@ -1392,7 +1400,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hiperligação" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1555,7 +1563,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2385,10 +2393,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E62CEF3-4F99-4CE5-B31F-511FA523F4D9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2418,7 +2427,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>215</v>
       </c>
@@ -2438,7 +2447,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>215</v>
       </c>
@@ -2458,7 +2467,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>215</v>
       </c>
@@ -2478,7 +2487,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>215</v>
       </c>
@@ -2495,7 +2504,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>215</v>
       </c>
@@ -2512,7 +2521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>215</v>
       </c>
@@ -2529,7 +2538,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>215</v>
       </c>
@@ -2546,7 +2555,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>215</v>
       </c>
@@ -2563,7 +2572,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>215</v>
       </c>
@@ -2580,7 +2589,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>215</v>
       </c>
@@ -2667,7 +2676,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -2684,7 +2693,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>215</v>
       </c>
@@ -2698,7 +2707,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>215</v>
       </c>
@@ -2715,7 +2724,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>215</v>
       </c>
@@ -2732,7 +2741,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>215</v>
       </c>
@@ -2749,7 +2758,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -2766,7 +2775,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>215</v>
       </c>
@@ -2783,7 +2792,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -2800,7 +2809,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -2817,7 +2826,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>215</v>
       </c>
@@ -2834,7 +2843,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>215</v>
       </c>
@@ -2851,7 +2860,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -2868,7 +2877,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -2885,7 +2894,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -2902,7 +2911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -3003,7 +3012,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>215</v>
       </c>
@@ -3020,7 +3029,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>215</v>
       </c>
@@ -3037,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>215</v>
       </c>
@@ -3054,7 +3063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>215</v>
       </c>
@@ -3071,7 +3080,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>215</v>
       </c>
@@ -3088,7 +3097,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>215</v>
       </c>
@@ -3105,7 +3114,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>215</v>
       </c>
@@ -3122,7 +3131,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>215</v>
       </c>
@@ -3139,7 +3148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>215</v>
       </c>
@@ -3156,7 +3165,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>215</v>
       </c>
@@ -3173,7 +3182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>215</v>
       </c>
@@ -3190,7 +3199,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>215</v>
       </c>
@@ -3207,7 +3216,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>215</v>
       </c>
@@ -3224,7 +3233,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>215</v>
       </c>
@@ -3241,7 +3250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>215</v>
       </c>
@@ -3258,7 +3267,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>215</v>
       </c>
@@ -3275,7 +3284,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>215</v>
       </c>
@@ -3292,7 +3301,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>215</v>
       </c>
@@ -3379,7 +3388,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>215</v>
       </c>
@@ -3393,7 +3402,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>215</v>
       </c>
@@ -3410,7 +3419,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -3427,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>215</v>
       </c>
@@ -3444,7 +3453,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -3461,7 +3470,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>215</v>
       </c>
@@ -3478,7 +3487,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>215</v>
       </c>
@@ -3495,7 +3504,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>215</v>
       </c>
@@ -3512,7 +3521,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>215</v>
       </c>
@@ -3529,7 +3538,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>215</v>
       </c>
@@ -3546,7 +3555,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -3563,7 +3572,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -3580,7 +3589,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>215</v>
       </c>
@@ -3653,7 +3662,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>215</v>
       </c>
@@ -3670,7 +3679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>215</v>
       </c>
@@ -3687,7 +3696,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>215</v>
       </c>
@@ -3704,7 +3713,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>215</v>
       </c>
@@ -3721,7 +3730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>215</v>
       </c>
@@ -3738,7 +3747,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>215</v>
       </c>
@@ -3755,7 +3764,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>215</v>
       </c>
@@ -3772,7 +3781,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>215</v>
       </c>
@@ -3845,7 +3854,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>215</v>
       </c>
@@ -3862,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -3879,7 +3888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>215</v>
       </c>
@@ -3896,7 +3905,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>215</v>
       </c>
@@ -3927,7 +3936,7 @@
         <v>44365</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>215</v>
       </c>
@@ -3944,7 +3953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>215</v>
       </c>
@@ -3961,7 +3970,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>215</v>
       </c>
@@ -4021,7 +4030,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E100" xr:uid="{9E62CEF3-4F99-4CE5-B31F-511FA523F4D9}"/>
+  <autoFilter ref="A1:E100" xr:uid="{9E62CEF3-4F99-4CE5-B31F-511FA523F4D9}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Finished"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B94:B97">
     <sortCondition ref="B94:B97"/>
   </sortState>
@@ -6246,8 +6261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC3EF37-2BA8-4EC6-92A1-22C0C9AA6791}">
   <dimension ref="A1:O67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6259,6 +6274,7 @@
     <col min="5" max="5" width="12.33203125" style="19" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.109375" style="10" customWidth="1"/>
     <col min="7" max="7" width="27.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -6286,6 +6302,9 @@
       <c r="H1" s="10" t="s">
         <v>332</v>
       </c>
+      <c r="I1" s="10" t="s">
+        <v>400</v>
+      </c>
       <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
@@ -6315,6 +6334,9 @@
       <c r="H2" s="26" t="s">
         <v>304</v>
       </c>
+      <c r="I2" s="26" t="s">
+        <v>401</v>
+      </c>
       <c r="O2" t="s">
         <v>85</v>
       </c>
@@ -6342,6 +6364,7 @@
         <v>335</v>
       </c>
       <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
       <c r="O3" t="s">
         <v>84</v>
       </c>
@@ -6369,6 +6392,7 @@
         <v>336</v>
       </c>
       <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
       <c r="O4" t="s">
         <v>87</v>
       </c>
@@ -6396,6 +6420,7 @@
         <v>337</v>
       </c>
       <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
@@ -6420,6 +6445,7 @@
         <v>338</v>
       </c>
       <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
@@ -6444,6 +6470,7 @@
         <v>339</v>
       </c>
       <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
@@ -6470,6 +6497,7 @@
       <c r="H8" s="26" t="s">
         <v>304</v>
       </c>
+      <c r="I8" s="26"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
@@ -6494,6 +6522,7 @@
         <v>341</v>
       </c>
       <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
@@ -6518,6 +6547,7 @@
         <v>342</v>
       </c>
       <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
@@ -6542,6 +6572,7 @@
         <v>343</v>
       </c>
       <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
@@ -6566,6 +6597,7 @@
         <v>344</v>
       </c>
       <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
@@ -6590,6 +6622,7 @@
         <v>345</v>
       </c>
       <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
@@ -6614,6 +6647,7 @@
         <v>346</v>
       </c>
       <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
@@ -6638,6 +6672,7 @@
         <v>347</v>
       </c>
       <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
@@ -6662,8 +6697,9 @@
         <v>348</v>
       </c>
       <c r="H16" s="13"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I16" s="13"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>215</v>
       </c>
@@ -6686,8 +6722,9 @@
         <v>349</v>
       </c>
       <c r="H17" s="13"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I17" s="13"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>215</v>
       </c>
@@ -6710,8 +6747,9 @@
         <v>350</v>
       </c>
       <c r="H18" s="13"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I18" s="13"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>215</v>
       </c>
@@ -6734,8 +6772,9 @@
         <v>351</v>
       </c>
       <c r="H19" s="13"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I19" s="13"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>215</v>
       </c>
@@ -6758,8 +6797,9 @@
         <v>352</v>
       </c>
       <c r="H20" s="13"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I20" s="13"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>215</v>
       </c>
@@ -6782,8 +6822,9 @@
         <v>353</v>
       </c>
       <c r="H21" s="13"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I21" s="13"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
@@ -6806,8 +6847,9 @@
         <v>354</v>
       </c>
       <c r="H22" s="13"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I22" s="13"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>215</v>
       </c>
@@ -6830,8 +6872,9 @@
         <v>355</v>
       </c>
       <c r="H23" s="13"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I23" s="13"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>215</v>
       </c>
@@ -6854,8 +6897,9 @@
         <v>356</v>
       </c>
       <c r="H24" s="13"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I24" s="13"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>215</v>
       </c>
@@ -6878,8 +6922,9 @@
         <v>357</v>
       </c>
       <c r="H25" s="13"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I25" s="13"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>215</v>
       </c>
@@ -6902,8 +6947,9 @@
         <v>358</v>
       </c>
       <c r="H26" s="13"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I26" s="13"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>215</v>
       </c>
@@ -6926,8 +6972,9 @@
         <v>359</v>
       </c>
       <c r="H27" s="13"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I27" s="13"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>215</v>
       </c>
@@ -6950,8 +6997,9 @@
         <v>360</v>
       </c>
       <c r="H28" s="13"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I28" s="13"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>215</v>
       </c>
@@ -6974,8 +7022,9 @@
         <v>361</v>
       </c>
       <c r="H29" s="13"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I29" s="13"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>215</v>
       </c>
@@ -6998,8 +7047,9 @@
         <v>362</v>
       </c>
       <c r="H30" s="13"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I30" s="13"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>215</v>
       </c>
@@ -7022,8 +7072,9 @@
         <v>363</v>
       </c>
       <c r="H31" s="13"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I31" s="13"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="25" t="s">
         <v>216</v>
       </c>
@@ -7046,8 +7097,9 @@
         <v>364</v>
       </c>
       <c r="H32" s="13"/>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I32" s="13"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>216</v>
       </c>
@@ -7070,8 +7122,9 @@
         <v>365</v>
       </c>
       <c r="H33" s="13"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I33" s="13"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>216</v>
       </c>
@@ -7094,8 +7147,9 @@
         <v>366</v>
       </c>
       <c r="H34" s="13"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I34" s="13"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>216</v>
       </c>
@@ -7118,8 +7172,9 @@
         <v>367</v>
       </c>
       <c r="H35" s="13"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I35" s="13"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>216</v>
       </c>
@@ -7142,8 +7197,9 @@
         <v>368</v>
       </c>
       <c r="H36" s="13"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I36" s="13"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>216</v>
       </c>
@@ -7166,8 +7222,9 @@
         <v>369</v>
       </c>
       <c r="H37" s="13"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I37" s="13"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>216</v>
       </c>
@@ -7190,8 +7247,9 @@
         <v>370</v>
       </c>
       <c r="H38" s="13"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I38" s="13"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>216</v>
       </c>
@@ -7214,8 +7272,9 @@
         <v>371</v>
       </c>
       <c r="H39" s="13"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I39" s="13"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>216</v>
       </c>
@@ -7238,8 +7297,9 @@
         <v>372</v>
       </c>
       <c r="H40" s="13"/>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I40" s="13"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>216</v>
       </c>
@@ -7264,8 +7324,9 @@
       <c r="H41" s="26" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I41" s="26"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>216</v>
       </c>
@@ -7287,9 +7348,14 @@
       <c r="G42" s="25" t="s">
         <v>374</v>
       </c>
-      <c r="H42" s="13"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H42" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I42" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>216</v>
       </c>
@@ -7311,9 +7377,14 @@
       <c r="G43" s="25" t="s">
         <v>375</v>
       </c>
-      <c r="H43" s="13"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H43" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I43" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>216</v>
       </c>
@@ -7335,9 +7406,14 @@
       <c r="G44" s="25" t="s">
         <v>376</v>
       </c>
-      <c r="H44" s="13"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H44" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I44" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>216</v>
       </c>
@@ -7359,9 +7435,14 @@
       <c r="G45" s="25" t="s">
         <v>377</v>
       </c>
-      <c r="H45" s="13"/>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H45" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I45" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>216</v>
       </c>
@@ -7383,9 +7464,14 @@
       <c r="G46" s="25" t="s">
         <v>378</v>
       </c>
-      <c r="H46" s="13"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H46" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I46" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>216</v>
       </c>
@@ -7407,9 +7493,14 @@
       <c r="G47" s="25" t="s">
         <v>379</v>
       </c>
-      <c r="H47" s="13"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H47" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I47" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>216</v>
       </c>
@@ -7431,9 +7522,14 @@
       <c r="G48" s="25" t="s">
         <v>380</v>
       </c>
-      <c r="H48" s="13"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I48" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>216</v>
       </c>
@@ -7455,9 +7551,14 @@
       <c r="G49" s="25" t="s">
         <v>381</v>
       </c>
-      <c r="H49" s="13"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H49" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I49" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>216</v>
       </c>
@@ -7479,9 +7580,14 @@
       <c r="G50" s="25" t="s">
         <v>382</v>
       </c>
-      <c r="H50" s="13"/>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H50" s="26" t="s">
+        <v>304</v>
+      </c>
+      <c r="I50" s="26" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>216</v>
       </c>
@@ -7504,8 +7610,9 @@
         <v>383</v>
       </c>
       <c r="H51" s="13"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I51" s="13"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>216</v>
       </c>
@@ -7528,8 +7635,9 @@
         <v>384</v>
       </c>
       <c r="H52" s="13"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I52" s="13"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>216</v>
       </c>
@@ -7552,8 +7660,9 @@
         <v>385</v>
       </c>
       <c r="H53" s="13"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I53" s="13"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>216</v>
       </c>
@@ -7576,8 +7685,9 @@
         <v>386</v>
       </c>
       <c r="H54" s="13"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I54" s="13"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>216</v>
       </c>
@@ -7600,8 +7710,9 @@
         <v>387</v>
       </c>
       <c r="H55" s="13"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I55" s="13"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>216</v>
       </c>
@@ -7624,8 +7735,9 @@
         <v>388</v>
       </c>
       <c r="H56" s="13"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>216</v>
       </c>
@@ -7648,8 +7760,9 @@
         <v>389</v>
       </c>
       <c r="H57" s="13"/>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I57" s="13"/>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>216</v>
       </c>
@@ -7672,8 +7785,9 @@
         <v>390</v>
       </c>
       <c r="H58" s="13"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I58" s="13"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>216</v>
       </c>
@@ -7696,8 +7810,9 @@
         <v>391</v>
       </c>
       <c r="H59" s="13"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I59" s="13"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>216</v>
       </c>
@@ -7720,8 +7835,9 @@
         <v>392</v>
       </c>
       <c r="H60" s="13"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I60" s="13"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>216</v>
       </c>
@@ -7744,8 +7860,9 @@
         <v>393</v>
       </c>
       <c r="H61" s="13"/>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I61" s="13"/>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>216</v>
       </c>
@@ -7768,8 +7885,9 @@
         <v>394</v>
       </c>
       <c r="H62" s="13"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I62" s="13"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>216</v>
       </c>
@@ -7792,8 +7910,9 @@
         <v>395</v>
       </c>
       <c r="H63" s="13"/>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I63" s="13"/>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>216</v>
       </c>
@@ -7816,8 +7935,9 @@
         <v>396</v>
       </c>
       <c r="H64" s="13"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I64" s="13"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>216</v>
       </c>
@@ -7840,8 +7960,9 @@
         <v>397</v>
       </c>
       <c r="H65" s="13"/>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I65" s="13"/>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>216</v>
       </c>
@@ -7864,8 +7985,9 @@
         <v>398</v>
       </c>
       <c r="H66" s="13"/>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="I66" s="13"/>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>216</v>
       </c>
@@ -7890,8 +8012,10 @@
       <c r="H67" s="26" t="s">
         <v>331</v>
       </c>
+      <c r="I67" s="26"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I67" xr:uid="{EDC3EF37-2BA8-4EC6-92A1-22C0C9AA6791}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F67" xr:uid="{A0E105BA-CF51-4401-B710-6BE9E69B1788}">
@@ -7904,12 +8028,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8116,15 +8237,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8149,10 +8274,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
US031: Refactoring: Task aggregate: (addresses #265) Design: Update CD and SD (addresses #257)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\switch\projectg2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B453E981-3115-4D9E-A144-5BB13B24889A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B65AC9-02EF-4190-BAC1-2381C4ABF416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6540" yWindow="2880" windowWidth="22114" windowHeight="8520" tabRatio="938" activeTab="5" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="938" activeTab="8" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1195" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="412">
   <si>
     <t>id</t>
   </si>
@@ -1281,6 +1281,12 @@
   </si>
   <si>
     <t>2021-04-02</t>
+  </si>
+  <si>
+    <t>A3 dummy 001</t>
+  </si>
+  <si>
+    <t>Project_2022_3&amp;as want US001</t>
   </si>
 </sst>
 </file>
@@ -1892,23 +1898,23 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3046875" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" customWidth="1"/>
-    <col min="5" max="5" width="19.765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.84375" style="4"/>
-    <col min="9" max="9" width="24.84375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.4609375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.69140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.69140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.84375" style="4"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="24.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="4"/>
     <col min="14" max="14" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>203</v>
       </c>
@@ -1952,7 +1958,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1994,7 +2000,7 @@
         <v>263650670</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -2036,7 +2042,7 @@
         <v>263650520</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -2078,7 +2084,7 @@
         <v>263650532</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -2120,7 +2126,7 @@
         <v>263650345</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -2162,7 +2168,7 @@
         <v>263650127</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>28</v>
       </c>
@@ -2204,7 +2210,7 @@
         <v>212349016</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
@@ -2228,7 +2234,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
@@ -2252,7 +2258,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>35</v>
       </c>
@@ -2276,7 +2282,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>37</v>
       </c>
@@ -2300,7 +2306,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>40</v>
       </c>
@@ -2324,7 +2330,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>41</v>
       </c>
@@ -2348,7 +2354,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
@@ -2372,7 +2378,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
@@ -2426,14 +2432,14 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2453,7 +2459,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>215</v>
       </c>
@@ -2473,7 +2479,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>215</v>
       </c>
@@ -2493,7 +2499,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>215</v>
       </c>
@@ -2513,7 +2519,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>215</v>
       </c>
@@ -2530,7 +2536,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>215</v>
       </c>
@@ -2547,7 +2553,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>215</v>
       </c>
@@ -2564,7 +2570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>215</v>
       </c>
@@ -2581,7 +2587,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>215</v>
       </c>
@@ -2598,7 +2604,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>215</v>
       </c>
@@ -2615,7 +2621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>215</v>
       </c>
@@ -2632,7 +2638,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>215</v>
       </c>
@@ -2646,7 +2652,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -2660,7 +2666,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -2674,7 +2680,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>215</v>
       </c>
@@ -2688,7 +2694,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>215</v>
       </c>
@@ -2702,7 +2708,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -2719,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>215</v>
       </c>
@@ -2733,7 +2739,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>215</v>
       </c>
@@ -2750,7 +2756,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>215</v>
       </c>
@@ -2767,7 +2773,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>215</v>
       </c>
@@ -2784,7 +2790,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -2801,7 +2807,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>215</v>
       </c>
@@ -2818,7 +2824,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -2835,7 +2841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -2852,7 +2858,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>215</v>
       </c>
@@ -2869,7 +2875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>215</v>
       </c>
@@ -2886,7 +2892,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -2903,7 +2909,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -2920,7 +2926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -2937,7 +2943,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -2954,7 +2960,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>215</v>
       </c>
@@ -2968,7 +2974,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>215</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>215</v>
       </c>
@@ -2996,7 +3002,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>215</v>
       </c>
@@ -3010,7 +3016,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>215</v>
       </c>
@@ -3024,7 +3030,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>215</v>
       </c>
@@ -3038,7 +3044,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>215</v>
       </c>
@@ -3055,7 +3061,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>215</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>215</v>
       </c>
@@ -3089,7 +3095,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>215</v>
       </c>
@@ -3106,7 +3112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>215</v>
       </c>
@@ -3123,7 +3129,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>215</v>
       </c>
@@ -3140,7 +3146,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>215</v>
       </c>
@@ -3157,7 +3163,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>215</v>
       </c>
@@ -3174,7 +3180,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>215</v>
       </c>
@@ -3191,7 +3197,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>215</v>
       </c>
@@ -3208,7 +3214,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>215</v>
       </c>
@@ -3225,7 +3231,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>215</v>
       </c>
@@ -3242,7 +3248,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>215</v>
       </c>
@@ -3259,7 +3265,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>215</v>
       </c>
@@ -3276,7 +3282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>215</v>
       </c>
@@ -3293,7 +3299,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>215</v>
       </c>
@@ -3310,7 +3316,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>215</v>
       </c>
@@ -3327,7 +3333,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>215</v>
       </c>
@@ -3344,7 +3350,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -3358,7 +3364,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>215</v>
       </c>
@@ -3372,7 +3378,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>215</v>
       </c>
@@ -3386,7 +3392,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>215</v>
       </c>
@@ -3400,7 +3406,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>215</v>
       </c>
@@ -3414,7 +3420,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>215</v>
       </c>
@@ -3428,7 +3434,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>215</v>
       </c>
@@ -3445,7 +3451,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -3462,7 +3468,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>215</v>
       </c>
@@ -3479,7 +3485,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -3496,7 +3502,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>215</v>
       </c>
@@ -3513,7 +3519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>215</v>
       </c>
@@ -3530,7 +3536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>215</v>
       </c>
@@ -3547,7 +3553,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>215</v>
       </c>
@@ -3564,7 +3570,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>215</v>
       </c>
@@ -3581,7 +3587,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -3598,7 +3604,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -3615,7 +3621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>215</v>
       </c>
@@ -3632,7 +3638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>215</v>
       </c>
@@ -3646,7 +3652,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>215</v>
       </c>
@@ -3660,7 +3666,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>215</v>
       </c>
@@ -3674,7 +3680,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>215</v>
       </c>
@@ -3688,7 +3694,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>215</v>
       </c>
@@ -3705,7 +3711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>215</v>
       </c>
@@ -3722,7 +3728,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>215</v>
       </c>
@@ -3739,7 +3745,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>215</v>
       </c>
@@ -3756,7 +3762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>215</v>
       </c>
@@ -3773,7 +3779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>215</v>
       </c>
@@ -3790,7 +3796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>215</v>
       </c>
@@ -3807,7 +3813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>215</v>
       </c>
@@ -3824,7 +3830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>215</v>
       </c>
@@ -3838,7 +3844,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>215</v>
       </c>
@@ -3852,7 +3858,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>215</v>
       </c>
@@ -3866,7 +3872,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>215</v>
       </c>
@@ -3880,7 +3886,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>215</v>
       </c>
@@ -3897,7 +3903,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -3914,7 +3920,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>215</v>
       </c>
@@ -3931,7 +3937,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>215</v>
       </c>
@@ -3948,7 +3954,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>215</v>
       </c>
@@ -3962,7 +3968,7 @@
         <v>44365</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>215</v>
       </c>
@@ -3979,7 +3985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>215</v>
       </c>
@@ -3996,7 +4002,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>215</v>
       </c>
@@ -4013,7 +4019,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>215</v>
       </c>
@@ -4027,7 +4033,7 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>215</v>
       </c>
@@ -4041,7 +4047,7 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>215</v>
       </c>
@@ -4078,17 +4084,17 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.07421875" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>227</v>
       </c>
@@ -4105,7 +4111,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -4123,7 +4129,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -4141,7 +4147,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -4159,7 +4165,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -4174,7 +4180,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -4189,7 +4195,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -4204,7 +4210,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -4219,7 +4225,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -4234,7 +4240,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>215</v>
       </c>
@@ -4249,7 +4255,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>215</v>
       </c>
@@ -4264,7 +4270,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>215</v>
       </c>
@@ -4279,7 +4285,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>215</v>
       </c>
@@ -4294,7 +4300,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>215</v>
       </c>
@@ -4309,7 +4315,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>215</v>
       </c>
@@ -4324,7 +4330,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>215</v>
       </c>
@@ -4339,7 +4345,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>215</v>
       </c>
@@ -4354,7 +4360,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>215</v>
       </c>
@@ -4369,7 +4375,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>215</v>
       </c>
@@ -4384,7 +4390,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>215</v>
       </c>
@@ -4399,7 +4405,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>215</v>
       </c>
@@ -4414,7 +4420,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
@@ -4429,7 +4435,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>215</v>
       </c>
@@ -4444,7 +4450,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>215</v>
       </c>
@@ -4459,7 +4465,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>215</v>
       </c>
@@ -4474,7 +4480,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>215</v>
       </c>
@@ -4489,7 +4495,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>215</v>
       </c>
@@ -4504,7 +4510,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>215</v>
       </c>
@@ -4519,7 +4525,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>215</v>
       </c>
@@ -4534,7 +4540,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>215</v>
       </c>
@@ -4549,7 +4555,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>215</v>
       </c>
@@ -4564,7 +4570,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>215</v>
       </c>
@@ -4579,7 +4585,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>215</v>
       </c>
@@ -4594,7 +4600,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>215</v>
       </c>
@@ -4609,7 +4615,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>215</v>
       </c>
@@ -4644,18 +4650,18 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.07421875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -4705,7 +4711,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U2" t="s">
         <v>183</v>
       </c>
@@ -4713,7 +4719,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U3" t="s">
         <v>184</v>
       </c>
@@ -4721,7 +4727,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U4" t="s">
         <v>186</v>
       </c>
@@ -4729,7 +4735,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U5" t="s">
         <v>187</v>
       </c>
@@ -4737,7 +4743,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U6" t="s">
         <v>189</v>
       </c>
@@ -4745,12 +4751,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U8" t="s">
         <v>191</v>
       </c>
@@ -4776,13 +4782,13 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.07421875" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" style="4"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -4790,7 +4796,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>45</v>
       </c>
@@ -4798,7 +4804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>46</v>
       </c>
@@ -4806,7 +4812,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
@@ -4814,7 +4820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>48</v>
       </c>
@@ -4836,17 +4842,17 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.07421875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" style="4"/>
-    <col min="4" max="4" width="7.3046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.53515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4866,7 +4872,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
@@ -4887,7 +4893,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>195</v>
       </c>
@@ -4908,7 +4914,7 @@
         <v>44198</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>192</v>
       </c>
@@ -4929,7 +4935,7 @@
         <v>44199</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>193</v>
       </c>
@@ -4950,7 +4956,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>194</v>
       </c>
@@ -4971,7 +4977,7 @@
         <v>44201</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>196</v>
       </c>
@@ -4992,7 +4998,7 @@
         <v>44567</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>32</v>
       </c>
@@ -5013,7 +5019,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>197</v>
       </c>
@@ -5034,7 +5040,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
@@ -5055,7 +5061,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -5076,7 +5082,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>198</v>
       </c>
@@ -5097,7 +5103,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>199</v>
       </c>
@@ -5118,7 +5124,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>200</v>
       </c>
@@ -5139,7 +5145,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>201</v>
       </c>
@@ -5160,11 +5166,11 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
     </row>
@@ -5198,24 +5204,24 @@
       <selection activeCell="D11" sqref="D11:Q12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3046875" customWidth="1"/>
-    <col min="7" max="7" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.84375" customWidth="1"/>
-    <col min="9" max="9" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -5256,7 +5262,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -5305,7 +5311,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>216</v>
       </c>
@@ -5354,7 +5360,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>217</v>
       </c>
@@ -5401,7 +5407,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -5441,15 +5447,15 @@
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.07421875" customWidth="1"/>
-    <col min="3" max="3" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -5463,7 +5469,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -5477,7 +5483,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -5491,7 +5497,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -5505,7 +5511,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -5519,7 +5525,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -5533,7 +5539,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>216</v>
       </c>
@@ -5547,7 +5553,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>216</v>
       </c>
@@ -5561,7 +5567,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>216</v>
       </c>
@@ -5572,7 +5578,7 @@
         <v>44354</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>216</v>
       </c>
@@ -5583,7 +5589,7 @@
         <v>44438</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>216</v>
       </c>
@@ -5594,7 +5600,7 @@
         <v>44627</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>216</v>
       </c>
@@ -5621,24 +5627,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8482F8C3-6DCA-424C-81AE-BDA1451F2AAD}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.53515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.84375" style="7"/>
-    <col min="9" max="9" width="9.23046875" style="7"/>
-    <col min="10" max="10" width="14.84375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="7"/>
+    <col min="9" max="9" width="9.21875" style="7"/>
+    <col min="10" max="10" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>218</v>
       </c>
@@ -5670,7 +5676,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>195</v>
       </c>
@@ -5703,7 +5709,7 @@
         <v>Tiago Cancado</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>192</v>
       </c>
@@ -5736,7 +5742,7 @@
         <v>Joao Silva</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>193</v>
       </c>
@@ -5769,7 +5775,7 @@
         <v>Manel Costa</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>194</v>
       </c>
@@ -5802,7 +5808,7 @@
         <v>Xico Ferreira</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -5835,7 +5841,7 @@
         <v>Nel Moleiro</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>197</v>
       </c>
@@ -5868,7 +5874,7 @@
         <v>Zé do Bento</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -5901,7 +5907,7 @@
         <v>Tó Farrulo</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
@@ -5934,7 +5940,7 @@
         <v>Tino das Cruzes</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>195</v>
       </c>
@@ -5967,7 +5973,7 @@
         <v>Tiago Cancado</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
         <v>192</v>
       </c>
@@ -6000,7 +6006,7 @@
         <v>Joao Silva</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
         <v>193</v>
       </c>
@@ -6033,7 +6039,7 @@
         <v>Manel Costa</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
         <v>194</v>
       </c>
@@ -6066,7 +6072,7 @@
         <v>Xico Ferreira</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
@@ -6099,7 +6105,7 @@
         <v>Nel Moleiro</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>197</v>
       </c>
@@ -6132,7 +6138,7 @@
         <v>Zé do Bento</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>36</v>
       </c>
@@ -6165,7 +6171,7 @@
         <v>Tó Farrulo</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>38</v>
       </c>
@@ -6207,20 +6213,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FF6538-20DF-4E13-8107-7AC155FD4D73}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>227</v>
       </c>
@@ -6231,7 +6237,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -6243,7 +6249,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -6255,7 +6261,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -6267,7 +6273,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -6279,7 +6285,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -6291,7 +6297,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -6303,7 +6309,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -6315,7 +6321,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -6327,7 +6333,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>216</v>
       </c>
@@ -6339,7 +6345,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>216</v>
       </c>
@@ -6351,7 +6357,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>216</v>
       </c>
@@ -6363,7 +6369,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>216</v>
       </c>
@@ -6375,7 +6381,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>216</v>
       </c>
@@ -6387,7 +6393,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>216</v>
       </c>
@@ -6399,7 +6405,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>216</v>
       </c>
@@ -6411,7 +6417,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>216</v>
       </c>
@@ -6423,7 +6429,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>216</v>
       </c>
@@ -6435,7 +6441,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>216</v>
       </c>
@@ -6447,7 +6453,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>216</v>
       </c>
@@ -6459,7 +6465,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>216</v>
       </c>
@@ -6469,6 +6475,18 @@
       </c>
       <c r="C21" s="10" t="s">
         <v>329</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B22" t="str">
+        <f>TEXT(1,"0")</f>
+        <v>1</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>406</v>
       </c>
     </row>
   </sheetData>
@@ -6485,13 +6503,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>203</v>
       </c>
@@ -6514,7 +6532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
@@ -6545,25 +6563,25 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC3EF37-2BA8-4EC6-92A1-22C0C9AA6791}">
-  <dimension ref="A1:O67"/>
+  <dimension ref="A1:O68"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" style="17"/>
-    <col min="4" max="4" width="15.84375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.3046875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.07421875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.53515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="17"/>
+    <col min="4" max="4" width="15.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>227</v>
       </c>
@@ -6595,7 +6613,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -6627,7 +6645,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -6655,7 +6673,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -6683,7 +6701,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -6708,7 +6726,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -6733,7 +6751,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -6758,7 +6776,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -6785,7 +6803,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -6810,7 +6828,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>215</v>
       </c>
@@ -6835,7 +6853,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>215</v>
       </c>
@@ -6860,7 +6878,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>215</v>
       </c>
@@ -6885,7 +6903,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>215</v>
       </c>
@@ -6910,7 +6928,7 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>215</v>
       </c>
@@ -6935,7 +6953,7 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>215</v>
       </c>
@@ -6960,7 +6978,7 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>215</v>
       </c>
@@ -6985,7 +7003,7 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>215</v>
       </c>
@@ -7010,7 +7028,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>215</v>
       </c>
@@ -7035,7 +7053,7 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>215</v>
       </c>
@@ -7060,7 +7078,7 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>215</v>
       </c>
@@ -7085,7 +7103,7 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>215</v>
       </c>
@@ -7110,7 +7128,7 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
@@ -7135,7 +7153,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>215</v>
       </c>
@@ -7160,7 +7178,7 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>215</v>
       </c>
@@ -7185,7 +7203,7 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>215</v>
       </c>
@@ -7210,7 +7228,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>215</v>
       </c>
@@ -7235,7 +7253,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>215</v>
       </c>
@@ -7260,7 +7278,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>215</v>
       </c>
@@ -7285,7 +7303,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>215</v>
       </c>
@@ -7310,7 +7328,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>215</v>
       </c>
@@ -7335,7 +7353,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>215</v>
       </c>
@@ -7360,7 +7378,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>216</v>
       </c>
@@ -7385,7 +7403,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>216</v>
       </c>
@@ -7410,7 +7428,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>216</v>
       </c>
@@ -7435,7 +7453,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>216</v>
       </c>
@@ -7464,7 +7482,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>216</v>
       </c>
@@ -7493,7 +7511,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>216</v>
       </c>
@@ -7522,7 +7540,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>216</v>
       </c>
@@ -7551,7 +7569,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>216</v>
       </c>
@@ -7580,7 +7598,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>216</v>
       </c>
@@ -7609,7 +7627,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>216</v>
       </c>
@@ -7638,7 +7656,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>216</v>
       </c>
@@ -7663,7 +7681,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>216</v>
       </c>
@@ -7688,7 +7706,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>216</v>
       </c>
@@ -7713,7 +7731,7 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>216</v>
       </c>
@@ -7738,7 +7756,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>216</v>
       </c>
@@ -7763,7 +7781,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>216</v>
       </c>
@@ -7788,7 +7806,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>216</v>
       </c>
@@ -7813,7 +7831,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>216</v>
       </c>
@@ -7838,7 +7856,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>216</v>
       </c>
@@ -7863,7 +7881,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>216</v>
       </c>
@@ -7888,7 +7906,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>216</v>
       </c>
@@ -7913,7 +7931,7 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>216</v>
       </c>
@@ -7938,7 +7956,7 @@
       <c r="H53" s="13"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>216</v>
       </c>
@@ -7963,7 +7981,7 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>216</v>
       </c>
@@ -7988,7 +8006,7 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>216</v>
       </c>
@@ -8013,7 +8031,7 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>216</v>
       </c>
@@ -8038,7 +8056,7 @@
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>216</v>
       </c>
@@ -8063,7 +8081,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>216</v>
       </c>
@@ -8088,7 +8106,7 @@
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>216</v>
       </c>
@@ -8113,7 +8131,7 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>216</v>
       </c>
@@ -8138,7 +8156,7 @@
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>216</v>
       </c>
@@ -8163,7 +8181,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>216</v>
       </c>
@@ -8188,7 +8206,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>216</v>
       </c>
@@ -8213,7 +8231,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>216</v>
       </c>
@@ -8238,7 +8256,7 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>216</v>
       </c>
@@ -8263,7 +8281,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>216</v>
       </c>
@@ -8291,11 +8309,36 @@
       <c r="I67" s="25" t="s">
         <v>331</v>
       </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="B68" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="C68" s="17">
+        <v>1</v>
+      </c>
+      <c r="D68" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="E68" s="18">
+        <v>26.5</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>411</v>
+      </c>
+      <c r="H68" s="13"/>
+      <c r="I68" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F67" xr:uid="{A0E105BA-CF51-4401-B710-6BE9E69B1788}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F68" xr:uid="{A0E105BA-CF51-4401-B710-6BE9E69B1788}">
       <formula1>$O$2:$O$4</formula1>
     </dataValidation>
   </dataValidations>
@@ -8305,9 +8348,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8514,19 +8560,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8551,9 +8593,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Implement: add records (us/sprint/tasks/efforts) to the data base (addresses #241)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\switch\projectg2\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B65AC9-02EF-4190-BAC1-2381C4ABF416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCC498-6C4D-445F-BABD-7A26CACB6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="938" activeTab="8" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView xWindow="2263" yWindow="2263" windowWidth="22114" windowHeight="8520" tabRatio="938" firstSheet="5" activeTab="13" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -25,9 +25,11 @@
     <sheet name="BacklogUSStatus" sheetId="12" r:id="rId10"/>
     <sheet name="SprintBacklog" sheetId="10" r:id="rId11"/>
     <sheet name="SprintTasks" sheetId="11" r:id="rId12"/>
+    <sheet name="Tasks" sheetId="14" r:id="rId13"/>
+    <sheet name="Efforts" sheetId="15" r:id="rId14"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId13"/>
+    <externalReference r:id="rId15"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">BacklogUSStatus!$A$1:$E$100</definedName>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="486">
   <si>
     <t>id</t>
   </si>
@@ -1287,6 +1289,228 @@
   </si>
   <si>
     <t>Project_2022_3&amp;as want US001</t>
+  </si>
+  <si>
+    <t>sprintName</t>
+  </si>
+  <si>
+    <t>resourceStartDate</t>
+  </si>
+  <si>
+    <t>taskTitle</t>
+  </si>
+  <si>
+    <t>taskDescription</t>
+  </si>
+  <si>
+    <t>taskEffortEstimate</t>
+  </si>
+  <si>
+    <t>taskType</t>
+  </si>
+  <si>
+    <t>ustittle</t>
+  </si>
+  <si>
+    <t>MEETING</t>
+  </si>
+  <si>
+    <t>2022-06-13</t>
+  </si>
+  <si>
+    <t>2022-03-21</t>
+  </si>
+  <si>
+    <t>2022-04-11</t>
+  </si>
+  <si>
+    <t>2022-05-02</t>
+  </si>
+  <si>
+    <t>2022-05-23</t>
+  </si>
+  <si>
+    <t>2022-07-04</t>
+  </si>
+  <si>
+    <t>2022-07-25</t>
+  </si>
+  <si>
+    <t>2022-08-15</t>
+  </si>
+  <si>
+    <t>2022-09-05</t>
+  </si>
+  <si>
+    <t>2022-09-26</t>
+  </si>
+  <si>
+    <t>2022-10-17</t>
+  </si>
+  <si>
+    <t>2022-11-07</t>
+  </si>
+  <si>
+    <t>2022-11-28</t>
+  </si>
+  <si>
+    <t>2023-01-02</t>
+  </si>
+  <si>
+    <t>Daily meeting</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>DESIGN</t>
+  </si>
+  <si>
+    <t>IMPLEMENTATION</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>createTaskSD</t>
+  </si>
+  <si>
+    <t>createTask</t>
+  </si>
+  <si>
+    <t>createTaskTest</t>
+  </si>
+  <si>
+    <t>Sequence Diagram</t>
+  </si>
+  <si>
+    <t>Implement</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>addUS_SD</t>
+  </si>
+  <si>
+    <t>addUS</t>
+  </si>
+  <si>
+    <t>addUSTest</t>
+  </si>
+  <si>
+    <t>DEPLOYMENT</t>
+  </si>
+  <si>
+    <t>deploy</t>
+  </si>
+  <si>
+    <t>sprint review</t>
+  </si>
+  <si>
+    <t>review</t>
+  </si>
+  <si>
+    <t>2022-06-24</t>
+  </si>
+  <si>
+    <t>Project_2022_3&amp;as want US002</t>
+  </si>
+  <si>
+    <t>Project_2022_3&amp;as want US003</t>
+  </si>
+  <si>
+    <t>A3 dummy 002</t>
+  </si>
+  <si>
+    <t>A3 dummy 003</t>
+  </si>
+  <si>
+    <t>sprint6</t>
+  </si>
+  <si>
+    <t>sprint1</t>
+  </si>
+  <si>
+    <t>sprint2</t>
+  </si>
+  <si>
+    <t>sprint3</t>
+  </si>
+  <si>
+    <t>sprint4</t>
+  </si>
+  <si>
+    <t>sprint5</t>
+  </si>
+  <si>
+    <t>sprint7</t>
+  </si>
+  <si>
+    <t>sprint8</t>
+  </si>
+  <si>
+    <t>sprint9</t>
+  </si>
+  <si>
+    <t>sprint10</t>
+  </si>
+  <si>
+    <t>sprint11</t>
+  </si>
+  <si>
+    <t>sprint12</t>
+  </si>
+  <si>
+    <t>sprint13</t>
+  </si>
+  <si>
+    <t>sprint14</t>
+  </si>
+  <si>
+    <t>sprint15</t>
+  </si>
+  <si>
+    <t>effortHours</t>
+  </si>
+  <si>
+    <t>effortMinutes</t>
+  </si>
+  <si>
+    <t>effortDate</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>attachment</t>
+  </si>
+  <si>
+    <t>2022-06-25</t>
+  </si>
+  <si>
+    <t>in schedule</t>
+  </si>
+  <si>
+    <t>Project_2022_3&amp;sprint6&amp;daily</t>
+  </si>
+  <si>
+    <t>note.pdf</t>
+  </si>
+  <si>
+    <t>define strategy</t>
+  </si>
+  <si>
+    <t>boardPhoto.pdf</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>snapshot.pdf</t>
+  </si>
+  <si>
+    <t>Project_2022_3&amp;as want US002&amp;createTaskSD</t>
   </si>
 </sst>
 </file>
@@ -1898,23 +2122,23 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="4"/>
-    <col min="9" max="9" width="24.88671875" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.3046875" customWidth="1"/>
+    <col min="3" max="3" width="15.84375" customWidth="1"/>
+    <col min="5" max="5" width="19.765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.84375" style="4"/>
+    <col min="9" max="9" width="24.84375" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.4609375" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.69140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.69140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.84375" style="4"/>
     <col min="14" max="14" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>203</v>
       </c>
@@ -1958,7 +2182,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -2000,7 +2224,7 @@
         <v>263650670</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -2042,7 +2266,7 @@
         <v>263650520</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -2084,7 +2308,7 @@
         <v>263650532</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -2126,7 +2350,7 @@
         <v>263650345</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -2168,7 +2392,7 @@
         <v>263650127</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>28</v>
       </c>
@@ -2210,7 +2434,7 @@
         <v>212349016</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
@@ -2234,7 +2458,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
@@ -2258,7 +2482,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>35</v>
       </c>
@@ -2282,7 +2506,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>37</v>
       </c>
@@ -2306,7 +2530,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>40</v>
       </c>
@@ -2330,7 +2554,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>41</v>
       </c>
@@ -2354,7 +2578,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
@@ -2378,7 +2602,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
@@ -2429,17 +2653,17 @@
   <dimension ref="A1:M100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2459,7 +2683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>215</v>
       </c>
@@ -2479,7 +2703,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>215</v>
       </c>
@@ -2499,7 +2723,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>215</v>
       </c>
@@ -2519,7 +2743,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>215</v>
       </c>
@@ -2536,7 +2760,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>215</v>
       </c>
@@ -2553,7 +2777,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
         <v>215</v>
       </c>
@@ -2570,7 +2794,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>215</v>
       </c>
@@ -2587,7 +2811,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>215</v>
       </c>
@@ -2604,7 +2828,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>215</v>
       </c>
@@ -2621,7 +2845,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>215</v>
       </c>
@@ -2638,7 +2862,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
         <v>215</v>
       </c>
@@ -2652,7 +2876,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -2666,7 +2890,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -2680,7 +2904,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
         <v>215</v>
       </c>
@@ -2694,7 +2918,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
         <v>215</v>
       </c>
@@ -2708,7 +2932,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -2725,7 +2949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18" t="s">
         <v>215</v>
       </c>
@@ -2739,7 +2963,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19" t="s">
         <v>215</v>
       </c>
@@ -2756,7 +2980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>215</v>
       </c>
@@ -2773,7 +2997,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21" t="s">
         <v>215</v>
       </c>
@@ -2790,7 +3014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -2807,7 +3031,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23" t="s">
         <v>215</v>
       </c>
@@ -2824,7 +3048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -2841,7 +3065,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -2858,7 +3082,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>215</v>
       </c>
@@ -2875,7 +3099,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A27" t="s">
         <v>215</v>
       </c>
@@ -2892,7 +3116,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -2909,7 +3133,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -2926,7 +3150,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -2943,7 +3167,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -2960,7 +3184,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>215</v>
       </c>
@@ -2974,7 +3198,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>215</v>
       </c>
@@ -2988,7 +3212,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
         <v>215</v>
       </c>
@@ -3002,7 +3226,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
         <v>215</v>
       </c>
@@ -3016,7 +3240,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>215</v>
       </c>
@@ -3030,7 +3254,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>215</v>
       </c>
@@ -3044,7 +3268,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>215</v>
       </c>
@@ -3061,7 +3285,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>215</v>
       </c>
@@ -3078,7 +3302,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
         <v>215</v>
       </c>
@@ -3095,7 +3319,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>215</v>
       </c>
@@ -3112,7 +3336,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>215</v>
       </c>
@@ -3129,7 +3353,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>215</v>
       </c>
@@ -3146,7 +3370,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>215</v>
       </c>
@@ -3163,7 +3387,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>215</v>
       </c>
@@ -3180,7 +3404,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>215</v>
       </c>
@@ -3197,7 +3421,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>215</v>
       </c>
@@ -3214,7 +3438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>215</v>
       </c>
@@ -3231,7 +3455,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>215</v>
       </c>
@@ -3248,7 +3472,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>215</v>
       </c>
@@ -3265,7 +3489,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>215</v>
       </c>
@@ -3282,7 +3506,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>215</v>
       </c>
@@ -3299,7 +3523,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>215</v>
       </c>
@@ -3316,7 +3540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>215</v>
       </c>
@@ -3333,7 +3557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>215</v>
       </c>
@@ -3350,7 +3574,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -3364,7 +3588,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57" t="s">
         <v>215</v>
       </c>
@@ -3378,7 +3602,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58" t="s">
         <v>215</v>
       </c>
@@ -3392,7 +3616,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A59" t="s">
         <v>215</v>
       </c>
@@ -3406,7 +3630,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A60" t="s">
         <v>215</v>
       </c>
@@ -3420,7 +3644,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A61" t="s">
         <v>215</v>
       </c>
@@ -3434,7 +3658,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A62" t="s">
         <v>215</v>
       </c>
@@ -3451,7 +3675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -3468,7 +3692,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64" t="s">
         <v>215</v>
       </c>
@@ -3485,7 +3709,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -3502,7 +3726,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A66" t="s">
         <v>215</v>
       </c>
@@ -3519,7 +3743,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A67" t="s">
         <v>215</v>
       </c>
@@ -3536,7 +3760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A68" t="s">
         <v>215</v>
       </c>
@@ -3553,7 +3777,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A69" t="s">
         <v>215</v>
       </c>
@@ -3570,7 +3794,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A70" t="s">
         <v>215</v>
       </c>
@@ -3587,7 +3811,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -3604,7 +3828,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -3621,7 +3845,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73" t="s">
         <v>215</v>
       </c>
@@ -3638,7 +3862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
         <v>215</v>
       </c>
@@ -3652,7 +3876,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
         <v>215</v>
       </c>
@@ -3666,7 +3890,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
         <v>215</v>
       </c>
@@ -3680,7 +3904,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77" s="3" t="s">
         <v>215</v>
       </c>
@@ -3694,7 +3918,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>215</v>
       </c>
@@ -3711,7 +3935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>215</v>
       </c>
@@ -3728,7 +3952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>215</v>
       </c>
@@ -3745,7 +3969,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>215</v>
       </c>
@@ -3762,7 +3986,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A82" s="3" t="s">
         <v>215</v>
       </c>
@@ -3779,7 +4003,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83" s="3" t="s">
         <v>215</v>
       </c>
@@ -3796,7 +4020,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>215</v>
       </c>
@@ -3813,7 +4037,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A85" s="3" t="s">
         <v>215</v>
       </c>
@@ -3830,7 +4054,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86" t="s">
         <v>215</v>
       </c>
@@ -3844,7 +4068,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A87" t="s">
         <v>215</v>
       </c>
@@ -3858,7 +4082,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88" t="s">
         <v>215</v>
       </c>
@@ -3872,7 +4096,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A89" t="s">
         <v>215</v>
       </c>
@@ -3886,7 +4110,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90" t="s">
         <v>215</v>
       </c>
@@ -3903,7 +4127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -3920,7 +4144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A92" t="s">
         <v>215</v>
       </c>
@@ -3937,7 +4161,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93" t="s">
         <v>215</v>
       </c>
@@ -3954,7 +4178,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A94" s="3" t="s">
         <v>215</v>
       </c>
@@ -3968,7 +4192,7 @@
         <v>44365</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>215</v>
       </c>
@@ -3985,7 +4209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A96" s="3" t="s">
         <v>215</v>
       </c>
@@ -4002,7 +4226,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97" s="3" t="s">
         <v>215</v>
       </c>
@@ -4019,7 +4243,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98" t="s">
         <v>215</v>
       </c>
@@ -4033,7 +4257,7 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A99" t="s">
         <v>215</v>
       </c>
@@ -4047,7 +4271,7 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A100" t="s">
         <v>215</v>
       </c>
@@ -4080,21 +4304,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62CAB123-B6B8-4C37-9FBC-A6CD32606951}">
   <dimension ref="A1:N35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.109375" customWidth="1"/>
+    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.07421875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>227</v>
       </c>
@@ -4111,7 +4335,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -4129,7 +4353,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -4147,7 +4371,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -4165,7 +4389,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -4180,7 +4404,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -4195,7 +4419,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -4210,7 +4434,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -4225,7 +4449,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -4240,7 +4464,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>215</v>
       </c>
@@ -4255,7 +4479,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>215</v>
       </c>
@@ -4270,7 +4494,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>215</v>
       </c>
@@ -4285,7 +4509,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>215</v>
       </c>
@@ -4300,7 +4524,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>215</v>
       </c>
@@ -4315,7 +4539,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>215</v>
       </c>
@@ -4330,7 +4554,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
         <v>215</v>
       </c>
@@ -4345,7 +4569,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
         <v>215</v>
       </c>
@@ -4360,7 +4584,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A18" s="10" t="s">
         <v>215</v>
       </c>
@@ -4375,7 +4599,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A19" s="10" t="s">
         <v>215</v>
       </c>
@@ -4390,7 +4614,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>215</v>
       </c>
@@ -4405,7 +4629,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>215</v>
       </c>
@@ -4420,7 +4644,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
@@ -4435,7 +4659,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>215</v>
       </c>
@@ -4450,7 +4674,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>215</v>
       </c>
@@ -4465,7 +4689,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>215</v>
       </c>
@@ -4480,7 +4704,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
         <v>215</v>
       </c>
@@ -4495,7 +4719,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>215</v>
       </c>
@@ -4510,7 +4734,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A28" s="10" t="s">
         <v>215</v>
       </c>
@@ -4525,7 +4749,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A29" s="10" t="s">
         <v>215</v>
       </c>
@@ -4540,7 +4764,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
         <v>215</v>
       </c>
@@ -4555,7 +4779,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A31" s="10" t="s">
         <v>215</v>
       </c>
@@ -4570,7 +4794,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A32" s="10" t="s">
         <v>215</v>
       </c>
@@ -4585,7 +4809,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A33" s="10" t="s">
         <v>215</v>
       </c>
@@ -4600,7 +4824,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A34" s="10" t="s">
         <v>215</v>
       </c>
@@ -4615,7 +4839,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A35" s="10" t="s">
         <v>215</v>
       </c>
@@ -4650,18 +4874,18 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.109375" customWidth="1"/>
+    <col min="9" max="9" width="12.07421875" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.3046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.84375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -4711,7 +4935,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
       <c r="U2" t="s">
         <v>183</v>
       </c>
@@ -4719,7 +4943,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
       <c r="U3" t="s">
         <v>184</v>
       </c>
@@ -4727,7 +4951,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
       <c r="U4" t="s">
         <v>186</v>
       </c>
@@ -4735,7 +4959,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
       <c r="U5" t="s">
         <v>187</v>
       </c>
@@ -4743,7 +4967,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
       <c r="U6" t="s">
         <v>189</v>
       </c>
@@ -4751,12 +4975,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
       <c r="U7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
       <c r="U8" t="s">
         <v>191</v>
       </c>
@@ -4774,6 +4998,438 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA25EC97-4F87-49A8-B3C7-E2A18A77C856}">
+  <dimension ref="A1:N10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.69140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.15234375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.23046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.3046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A2" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>435</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>434</v>
+      </c>
+      <c r="H2" s="18">
+        <v>4</v>
+      </c>
+      <c r="I2" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A3" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>439</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="H3" s="18">
+        <v>15</v>
+      </c>
+      <c r="I3" s="10" t="s">
+        <v>436</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A4" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>440</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="H4" s="18">
+        <v>30</v>
+      </c>
+      <c r="I4" s="10" t="s">
+        <v>437</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A5" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="H5" s="18">
+        <v>20</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>438</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A6" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>445</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="H6" s="18">
+        <v>7.5</v>
+      </c>
+      <c r="I6" s="10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A7" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>446</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="H7" s="18">
+        <v>15</v>
+      </c>
+      <c r="I7" s="10" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A8" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>447</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>444</v>
+      </c>
+      <c r="H8" s="18">
+        <v>10</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A9" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>449</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>191</v>
+      </c>
+      <c r="H9" s="18">
+        <v>4</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+      <c r="A10" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>406</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>451</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>450</v>
+      </c>
+      <c r="H10" s="18">
+        <v>4</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{BAF48CC2-26FD-46FF-9951-A42E1BAB59A1}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{D97BF529-3583-461E-9C47-16812B9A7808}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{931797C7-3760-442C-ACA9-010BAC442FD8}"/>
+    <hyperlink ref="D5" r:id="rId4" xr:uid="{A43BE419-EB66-42CD-A53E-5483DAE0B7A4}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{5CD5B1A3-4E23-4FFB-AEF0-D6A7DA389801}"/>
+    <hyperlink ref="D7" r:id="rId6" xr:uid="{76BD29EF-9EF3-43EB-AC20-721F79F8F708}"/>
+    <hyperlink ref="D8" r:id="rId7" xr:uid="{5622DCA8-B2E7-47FF-BF19-E3C0EA87C8AE}"/>
+    <hyperlink ref="D9" r:id="rId8" xr:uid="{3AF8B547-E50D-449C-A393-2F761C9AB110}"/>
+    <hyperlink ref="D10" r:id="rId9" xr:uid="{DE66F1F2-A7AF-4AD8-BF89-CF5313D75667}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA51A6B7-E36D-420E-A2B8-AD7FB5872218}">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.07421875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.3046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>476</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A2" s="17">
+        <v>2</v>
+      </c>
+      <c r="B2" s="17">
+        <v>30</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>481</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>482</v>
+      </c>
+      <c r="F2" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A3" s="17">
+        <v>0</v>
+      </c>
+      <c r="B3" s="17">
+        <v>30</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>477</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>480</v>
+      </c>
+      <c r="F3" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="17">
+        <v>15</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>483</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>484</v>
+      </c>
+      <c r="F4" t="s">
+        <v>485</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A13260C-C42D-4E60-BE2C-2CA24BC2C1E2}">
   <dimension ref="A1:B5"/>
@@ -4782,13 +5438,13 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.109375" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" style="4"/>
+    <col min="1" max="1" width="19.07421875" customWidth="1"/>
+    <col min="2" max="2" width="8.84375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -4796,7 +5452,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>45</v>
       </c>
@@ -4804,7 +5460,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>46</v>
       </c>
@@ -4812,7 +5468,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
@@ -4820,7 +5476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>48</v>
       </c>
@@ -4842,17 +5498,17 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="4"/>
-    <col min="4" max="4" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.07421875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" style="4"/>
+    <col min="4" max="4" width="7.3046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.3046875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.53515625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4872,7 +5528,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
@@ -4893,7 +5549,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" s="12" t="s">
         <v>195</v>
       </c>
@@ -4914,7 +5570,7 @@
         <v>44198</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
         <v>192</v>
       </c>
@@ -4935,7 +5591,7 @@
         <v>44199</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" s="12" t="s">
         <v>193</v>
       </c>
@@ -4956,7 +5612,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A6" s="12" t="s">
         <v>194</v>
       </c>
@@ -4977,7 +5633,7 @@
         <v>44201</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A7" s="12" t="s">
         <v>196</v>
       </c>
@@ -4998,7 +5654,7 @@
         <v>44567</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" s="12" t="s">
         <v>32</v>
       </c>
@@ -5019,7 +5675,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
         <v>197</v>
       </c>
@@ -5040,7 +5696,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
@@ -5061,7 +5717,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -5082,7 +5738,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A12" s="12" t="s">
         <v>198</v>
       </c>
@@ -5103,7 +5759,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A13" s="12" t="s">
         <v>199</v>
       </c>
@@ -5124,7 +5780,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A14" s="12" t="s">
         <v>200</v>
       </c>
@@ -5145,7 +5801,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A15" s="12" t="s">
         <v>201</v>
       </c>
@@ -5166,11 +5822,11 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
     </row>
@@ -5200,28 +5856,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D59AF7EF-B12B-4A6F-9425-B1B26B554B1A}">
   <dimension ref="A1:R5"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11:Q12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" customWidth="1"/>
-    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
-    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.53515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.3046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.69140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.3046875" customWidth="1"/>
+    <col min="7" max="7" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.84375" customWidth="1"/>
+    <col min="9" max="9" width="15.53515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.69140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.23046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.53515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.53515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -5262,7 +5918,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -5311,7 +5967,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>216</v>
       </c>
@@ -5360,7 +6016,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>217</v>
       </c>
@@ -5407,7 +6063,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -5444,18 +6100,18 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.07421875" customWidth="1"/>
+    <col min="3" max="3" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.3046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -5469,7 +6125,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -5483,7 +6139,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -5497,7 +6153,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -5511,7 +6167,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -5525,7 +6181,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -5539,7 +6195,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>216</v>
       </c>
@@ -5553,7 +6209,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>216</v>
       </c>
@@ -5567,7 +6223,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>216</v>
       </c>
@@ -5578,7 +6234,7 @@
         <v>44354</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>216</v>
       </c>
@@ -5589,7 +6245,7 @@
         <v>44438</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>216</v>
       </c>
@@ -5600,7 +6256,7 @@
         <v>44627</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>216</v>
       </c>
@@ -5631,20 +6287,20 @@
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="7"/>
-    <col min="9" max="9" width="9.21875" style="7"/>
-    <col min="10" max="10" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.53515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.53515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.07421875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.69140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.84375" style="7"/>
+    <col min="9" max="9" width="9.23046875" style="7"/>
+    <col min="10" max="10" width="14.84375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>218</v>
       </c>
@@ -5676,7 +6332,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>195</v>
       </c>
@@ -5709,7 +6365,7 @@
         <v>Tiago Cancado</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>192</v>
       </c>
@@ -5742,7 +6398,7 @@
         <v>Joao Silva</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>193</v>
       </c>
@@ -5775,7 +6431,7 @@
         <v>Manel Costa</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>194</v>
       </c>
@@ -5808,7 +6464,7 @@
         <v>Xico Ferreira</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -5841,7 +6497,7 @@
         <v>Nel Moleiro</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>197</v>
       </c>
@@ -5874,7 +6530,7 @@
         <v>Zé do Bento</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -5907,7 +6563,7 @@
         <v>Tó Farrulo</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
@@ -5940,7 +6596,7 @@
         <v>Tino das Cruzes</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A10" s="28" t="s">
         <v>195</v>
       </c>
@@ -5973,7 +6629,7 @@
         <v>Tiago Cancado</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="28" t="s">
         <v>192</v>
       </c>
@@ -6006,7 +6662,7 @@
         <v>Joao Silva</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="28" t="s">
         <v>193</v>
       </c>
@@ -6039,7 +6695,7 @@
         <v>Manel Costa</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="28" t="s">
         <v>194</v>
       </c>
@@ -6072,7 +6728,7 @@
         <v>Xico Ferreira</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
@@ -6105,7 +6761,7 @@
         <v>Nel Moleiro</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="28" t="s">
         <v>197</v>
       </c>
@@ -6138,7 +6794,7 @@
         <v>Zé do Bento</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="28" t="s">
         <v>36</v>
       </c>
@@ -6171,7 +6827,7 @@
         <v>Tó Farrulo</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="28" t="s">
         <v>38</v>
       </c>
@@ -6213,20 +6869,20 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FF6538-20DF-4E13-8107-7AC155FD4D73}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="19" t="s">
         <v>227</v>
       </c>
@@ -6237,7 +6893,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -6249,7 +6905,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -6261,7 +6917,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -6273,7 +6929,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -6285,7 +6941,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -6297,7 +6953,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -6309,7 +6965,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -6321,7 +6977,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -6333,7 +6989,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>216</v>
       </c>
@@ -6345,7 +7001,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>216</v>
       </c>
@@ -6357,7 +7013,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>216</v>
       </c>
@@ -6369,7 +7025,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>216</v>
       </c>
@@ -6381,7 +7037,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>216</v>
       </c>
@@ -6393,7 +7049,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>216</v>
       </c>
@@ -6405,7 +7061,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
         <v>216</v>
       </c>
@@ -6417,7 +7073,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
         <v>216</v>
       </c>
@@ -6429,7 +7085,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="10" t="s">
         <v>216</v>
       </c>
@@ -6441,7 +7097,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="10" t="s">
         <v>216</v>
       </c>
@@ -6453,7 +7109,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>216</v>
       </c>
@@ -6465,7 +7121,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>216</v>
       </c>
@@ -6477,16 +7133,169 @@
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="B22" t="str">
-        <f>TEXT(1,"0")</f>
-        <v>1</v>
+      <c r="B22" s="10" t="s">
+        <v>458</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>406</v>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A23" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>460</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A25" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A26" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>462</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A27" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A28" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>463</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A29" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>464</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A30" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>465</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A31" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>466</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A32" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>467</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A33" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>468</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A34" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>469</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A35" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>470</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A36" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>471</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>433</v>
       </c>
     </row>
   </sheetData>
@@ -6503,13 +7312,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.84375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C1" s="1" t="s">
         <v>203</v>
       </c>
@@ -6532,7 +7341,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.4">
       <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
@@ -6563,25 +7372,25 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC3EF37-2BA8-4EC6-92A1-22C0C9AA6791}">
-  <dimension ref="A1:O68"/>
+  <dimension ref="A1:O70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="17"/>
-    <col min="4" max="4" width="15.88671875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.84375" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.84375" style="17"/>
+    <col min="4" max="4" width="15.84375" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.3046875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.07421875" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.53515625" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
         <v>227</v>
       </c>
@@ -6613,7 +7422,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -6645,7 +7454,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -6673,7 +7482,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -6701,7 +7510,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -6726,7 +7535,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -6751,7 +7560,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -6776,7 +7585,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -6803,7 +7612,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -6828,7 +7637,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>215</v>
       </c>
@@ -6853,7 +7662,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>215</v>
       </c>
@@ -6878,7 +7687,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12" s="10" t="s">
         <v>215</v>
       </c>
@@ -6903,7 +7712,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13" s="10" t="s">
         <v>215</v>
       </c>
@@ -6928,7 +7737,7 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14" s="10" t="s">
         <v>215</v>
       </c>
@@ -6953,7 +7762,7 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15" s="10" t="s">
         <v>215</v>
       </c>
@@ -6978,7 +7787,7 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A16" s="10" t="s">
         <v>215</v>
       </c>
@@ -7003,7 +7812,7 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A17" s="10" t="s">
         <v>215</v>
       </c>
@@ -7028,7 +7837,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A18" s="10" t="s">
         <v>215</v>
       </c>
@@ -7053,7 +7862,7 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A19" s="10" t="s">
         <v>215</v>
       </c>
@@ -7078,7 +7887,7 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A20" s="10" t="s">
         <v>215</v>
       </c>
@@ -7103,7 +7912,7 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A21" s="10" t="s">
         <v>215</v>
       </c>
@@ -7128,7 +7937,7 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
@@ -7153,7 +7962,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A23" s="10" t="s">
         <v>215</v>
       </c>
@@ -7178,7 +7987,7 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A24" s="10" t="s">
         <v>215</v>
       </c>
@@ -7203,7 +8012,7 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A25" s="10" t="s">
         <v>215</v>
       </c>
@@ -7228,7 +8037,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A26" s="10" t="s">
         <v>215</v>
       </c>
@@ -7253,7 +8062,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A27" s="10" t="s">
         <v>215</v>
       </c>
@@ -7278,7 +8087,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A28" s="10" t="s">
         <v>215</v>
       </c>
@@ -7303,7 +8112,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A29" s="10" t="s">
         <v>215</v>
       </c>
@@ -7328,7 +8137,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A30" s="10" t="s">
         <v>215</v>
       </c>
@@ -7353,7 +8162,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A31" s="10" t="s">
         <v>215</v>
       </c>
@@ -7378,7 +8187,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A32" s="24" t="s">
         <v>216</v>
       </c>
@@ -7403,7 +8212,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A33" s="10" t="s">
         <v>216</v>
       </c>
@@ -7428,7 +8237,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A34" s="10" t="s">
         <v>216</v>
       </c>
@@ -7453,7 +8262,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A35" s="10" t="s">
         <v>216</v>
       </c>
@@ -7482,7 +8291,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A36" s="10" t="s">
         <v>216</v>
       </c>
@@ -7511,7 +8320,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A37" s="10" t="s">
         <v>216</v>
       </c>
@@ -7540,7 +8349,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A38" s="10" t="s">
         <v>216</v>
       </c>
@@ -7569,7 +8378,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A39" s="10" t="s">
         <v>216</v>
       </c>
@@ -7598,7 +8407,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A40" s="10" t="s">
         <v>216</v>
       </c>
@@ -7627,7 +8436,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A41" s="10" t="s">
         <v>216</v>
       </c>
@@ -7656,7 +8465,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A42" s="10" t="s">
         <v>216</v>
       </c>
@@ -7681,7 +8490,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A43" s="10" t="s">
         <v>216</v>
       </c>
@@ -7706,7 +8515,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A44" s="10" t="s">
         <v>216</v>
       </c>
@@ -7731,7 +8540,7 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A45" s="10" t="s">
         <v>216</v>
       </c>
@@ -7756,7 +8565,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A46" s="10" t="s">
         <v>216</v>
       </c>
@@ -7781,7 +8590,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A47" s="10" t="s">
         <v>216</v>
       </c>
@@ -7806,7 +8615,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A48" s="10" t="s">
         <v>216</v>
       </c>
@@ -7831,7 +8640,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" s="10" t="s">
         <v>216</v>
       </c>
@@ -7856,7 +8665,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" s="10" t="s">
         <v>216</v>
       </c>
@@ -7881,7 +8690,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" s="10" t="s">
         <v>216</v>
       </c>
@@ -7906,7 +8715,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" s="10" t="s">
         <v>216</v>
       </c>
@@ -7931,7 +8740,7 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" s="10" t="s">
         <v>216</v>
       </c>
@@ -7956,7 +8765,7 @@
       <c r="H53" s="13"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" s="10" t="s">
         <v>216</v>
       </c>
@@ -7981,7 +8790,7 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" s="10" t="s">
         <v>216</v>
       </c>
@@ -8006,7 +8815,7 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A56" s="10" t="s">
         <v>216</v>
       </c>
@@ -8031,7 +8840,7 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A57" s="10" t="s">
         <v>216</v>
       </c>
@@ -8056,7 +8865,7 @@
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A58" s="10" t="s">
         <v>216</v>
       </c>
@@ -8081,7 +8890,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A59" s="10" t="s">
         <v>216</v>
       </c>
@@ -8106,7 +8915,7 @@
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A60" s="10" t="s">
         <v>216</v>
       </c>
@@ -8131,7 +8940,7 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A61" s="10" t="s">
         <v>216</v>
       </c>
@@ -8156,7 +8965,7 @@
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A62" s="10" t="s">
         <v>216</v>
       </c>
@@ -8181,7 +8990,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A63" s="10" t="s">
         <v>216</v>
       </c>
@@ -8206,7 +9015,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A64" s="10" t="s">
         <v>216</v>
       </c>
@@ -8231,7 +9040,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A65" s="10" t="s">
         <v>216</v>
       </c>
@@ -8256,7 +9065,7 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A66" s="10" t="s">
         <v>216</v>
       </c>
@@ -8281,7 +9090,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A67" s="10" t="s">
         <v>216</v>
       </c>
@@ -8310,8 +9119,8 @@
         <v>331</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A68" s="24" t="s">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A68" s="10" t="s">
         <v>217</v>
       </c>
       <c r="B68" s="10" t="s">
@@ -8334,11 +9143,63 @@
       </c>
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A69" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>261</v>
+      </c>
+      <c r="C69" s="17">
+        <v>2</v>
+      </c>
+      <c r="D69" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="E69" s="18">
+        <v>70</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G69" s="24" t="s">
+        <v>453</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>452</v>
+      </c>
+      <c r="I69" s="13"/>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="A70" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="B70" s="10" t="s">
+        <v>262</v>
+      </c>
+      <c r="C70" s="17">
+        <v>3</v>
+      </c>
+      <c r="D70" s="10" t="s">
+        <v>456</v>
+      </c>
+      <c r="E70" s="18">
+        <v>35</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G70" s="24" t="s">
+        <v>454</v>
+      </c>
+      <c r="H70" s="10"/>
+      <c r="I70" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F68" xr:uid="{A0E105BA-CF51-4401-B710-6BE9E69B1788}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F70" xr:uid="{A0E105BA-CF51-4401-B710-6BE9E69B1788}">
       <formula1>$O$2:$O$4</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Improving test coverage. ProjectJPaAssembler test (addresses #182)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\switch\projectg2\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91e2d21952d024e0/Documentos/Switch/projectg2/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFCC498-6C4D-445F-BABD-7A26CACB6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{ADFCC498-6C4D-445F-BABD-7A26CACB6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{162A7242-D61A-409F-9361-2B9D8A5114E7}"/>
   <bookViews>
-    <workbookView xWindow="2263" yWindow="2263" windowWidth="22114" windowHeight="8520" tabRatio="938" firstSheet="5" activeTab="13" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView minimized="1" xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" tabRatio="938" firstSheet="2" activeTab="5" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">BacklogUSStatus!$A$1:$E$100</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ProjectBacklog!$A$1:$H$67</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +43,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -2122,23 +2124,23 @@
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.4609375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.3046875" customWidth="1"/>
-    <col min="3" max="3" width="15.84375" customWidth="1"/>
-    <col min="5" max="5" width="19.765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="15.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.84375" style="4"/>
-    <col min="9" max="9" width="24.84375" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.4609375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.69140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.69140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.84375" style="4"/>
+    <col min="1" max="1" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="4"/>
+    <col min="9" max="9" width="24.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.88671875" style="4"/>
     <col min="14" max="14" width="10" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>203</v>
       </c>
@@ -2182,7 +2184,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -2224,7 +2226,7 @@
         <v>263650670</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>19</v>
       </c>
@@ -2266,7 +2268,7 @@
         <v>263650520</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -2308,7 +2310,7 @@
         <v>263650532</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>23</v>
       </c>
@@ -2350,7 +2352,7 @@
         <v>263650345</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
@@ -2392,7 +2394,7 @@
         <v>263650127</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>28</v>
       </c>
@@ -2434,7 +2436,7 @@
         <v>212349016</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>31</v>
       </c>
@@ -2458,7 +2460,7 @@
         <v>1241</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>34</v>
       </c>
@@ -2482,7 +2484,7 @@
         <v>1243</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>35</v>
       </c>
@@ -2506,7 +2508,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>37</v>
       </c>
@@ -2530,7 +2532,7 @@
         <v>1247</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>40</v>
       </c>
@@ -2554,7 +2556,7 @@
         <v>1251</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>41</v>
       </c>
@@ -2578,7 +2580,7 @@
         <v>1252</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>42</v>
       </c>
@@ -2602,7 +2604,7 @@
         <v>1253</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>43</v>
       </c>
@@ -2656,14 +2658,14 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.53515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -2683,7 +2685,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>215</v>
       </c>
@@ -2703,7 +2705,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>215</v>
       </c>
@@ -2723,7 +2725,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>215</v>
       </c>
@@ -2743,7 +2745,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>215</v>
       </c>
@@ -2760,7 +2762,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>215</v>
       </c>
@@ -2777,7 +2779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>215</v>
       </c>
@@ -2794,7 +2796,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>215</v>
       </c>
@@ -2811,7 +2813,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>215</v>
       </c>
@@ -2828,7 +2830,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>215</v>
       </c>
@@ -2845,7 +2847,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>215</v>
       </c>
@@ -2862,7 +2864,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>215</v>
       </c>
@@ -2876,7 +2878,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>215</v>
       </c>
@@ -2890,7 +2892,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>215</v>
       </c>
@@ -2904,7 +2906,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>215</v>
       </c>
@@ -2918,7 +2920,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>215</v>
       </c>
@@ -2932,7 +2934,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>215</v>
       </c>
@@ -2949,7 +2951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>215</v>
       </c>
@@ -2963,7 +2965,7 @@
         <v>44288</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>215</v>
       </c>
@@ -2980,7 +2982,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>215</v>
       </c>
@@ -2997,7 +2999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>215</v>
       </c>
@@ -3014,7 +3016,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>215</v>
       </c>
@@ -3031,7 +3033,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>215</v>
       </c>
@@ -3048,7 +3050,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>215</v>
       </c>
@@ -3065,7 +3067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>215</v>
       </c>
@@ -3082,7 +3084,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>215</v>
       </c>
@@ -3099,7 +3101,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>215</v>
       </c>
@@ -3116,7 +3118,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>215</v>
       </c>
@@ -3133,7 +3135,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>215</v>
       </c>
@@ -3150,7 +3152,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>215</v>
       </c>
@@ -3167,7 +3169,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>215</v>
       </c>
@@ -3184,7 +3186,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>215</v>
       </c>
@@ -3198,7 +3200,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>215</v>
       </c>
@@ -3212,7 +3214,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>215</v>
       </c>
@@ -3226,7 +3228,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>215</v>
       </c>
@@ -3240,7 +3242,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>215</v>
       </c>
@@ -3254,7 +3256,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>215</v>
       </c>
@@ -3268,7 +3270,7 @@
         <v>44309</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>215</v>
       </c>
@@ -3285,7 +3287,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>215</v>
       </c>
@@ -3302,7 +3304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>215</v>
       </c>
@@ -3319,7 +3321,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>215</v>
       </c>
@@ -3336,7 +3338,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>215</v>
       </c>
@@ -3353,7 +3355,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>215</v>
       </c>
@@ -3370,7 +3372,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>215</v>
       </c>
@@ -3387,7 +3389,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>215</v>
       </c>
@@ -3404,7 +3406,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>215</v>
       </c>
@@ -3421,7 +3423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>215</v>
       </c>
@@ -3438,7 +3440,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>215</v>
       </c>
@@ -3455,7 +3457,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>215</v>
       </c>
@@ -3472,7 +3474,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>215</v>
       </c>
@@ -3489,7 +3491,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>215</v>
       </c>
@@ -3506,7 +3508,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>215</v>
       </c>
@@ -3523,7 +3525,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>215</v>
       </c>
@@ -3540,7 +3542,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>215</v>
       </c>
@@ -3557,7 +3559,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>215</v>
       </c>
@@ -3574,7 +3576,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>215</v>
       </c>
@@ -3588,7 +3590,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>215</v>
       </c>
@@ -3602,7 +3604,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>215</v>
       </c>
@@ -3616,7 +3618,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>215</v>
       </c>
@@ -3630,7 +3632,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>215</v>
       </c>
@@ -3644,7 +3646,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>215</v>
       </c>
@@ -3658,7 +3660,7 @@
         <v>44323</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>215</v>
       </c>
@@ -3675,7 +3677,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>215</v>
       </c>
@@ -3692,7 +3694,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>215</v>
       </c>
@@ -3709,7 +3711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>215</v>
       </c>
@@ -3726,7 +3728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>215</v>
       </c>
@@ -3743,7 +3745,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>215</v>
       </c>
@@ -3760,7 +3762,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>215</v>
       </c>
@@ -3777,7 +3779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>215</v>
       </c>
@@ -3794,7 +3796,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>215</v>
       </c>
@@ -3811,7 +3813,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>215</v>
       </c>
@@ -3828,7 +3830,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>215</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>215</v>
       </c>
@@ -3862,7 +3864,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>215</v>
       </c>
@@ -3876,7 +3878,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>215</v>
       </c>
@@ -3890,7 +3892,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>215</v>
       </c>
@@ -3904,7 +3906,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>215</v>
       </c>
@@ -3918,7 +3920,7 @@
         <v>44337</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>215</v>
       </c>
@@ -3935,7 +3937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>215</v>
       </c>
@@ -3952,7 +3954,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>215</v>
       </c>
@@ -3969,7 +3971,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>215</v>
       </c>
@@ -3986,7 +3988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>215</v>
       </c>
@@ -4003,7 +4005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>215</v>
       </c>
@@ -4020,7 +4022,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>215</v>
       </c>
@@ -4037,7 +4039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>215</v>
       </c>
@@ -4054,7 +4056,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>215</v>
       </c>
@@ -4068,7 +4070,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>215</v>
       </c>
@@ -4082,7 +4084,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>215</v>
       </c>
@@ -4096,7 +4098,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>215</v>
       </c>
@@ -4110,7 +4112,7 @@
         <v>44351</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>215</v>
       </c>
@@ -4127,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>215</v>
       </c>
@@ -4144,7 +4146,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>215</v>
       </c>
@@ -4161,7 +4163,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>215</v>
       </c>
@@ -4178,7 +4180,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>215</v>
       </c>
@@ -4192,7 +4194,7 @@
         <v>44365</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>215</v>
       </c>
@@ -4209,7 +4211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>215</v>
       </c>
@@ -4226,7 +4228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>215</v>
       </c>
@@ -4243,7 +4245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>215</v>
       </c>
@@ -4257,7 +4259,7 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>215</v>
       </c>
@@ -4271,7 +4273,7 @@
         <v>44407</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>215</v>
       </c>
@@ -4308,17 +4310,17 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.07421875" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>227</v>
       </c>
@@ -4335,7 +4337,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -4353,7 +4355,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -4371,7 +4373,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -4389,7 +4391,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -4404,7 +4406,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -4419,7 +4421,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -4434,7 +4436,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -4449,7 +4451,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -4464,7 +4466,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>215</v>
       </c>
@@ -4479,7 +4481,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>215</v>
       </c>
@@ -4494,7 +4496,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>215</v>
       </c>
@@ -4509,7 +4511,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>215</v>
       </c>
@@ -4524,7 +4526,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>215</v>
       </c>
@@ -4539,7 +4541,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>215</v>
       </c>
@@ -4554,7 +4556,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>215</v>
       </c>
@@ -4569,7 +4571,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>215</v>
       </c>
@@ -4584,7 +4586,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>215</v>
       </c>
@@ -4599,7 +4601,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>215</v>
       </c>
@@ -4614,7 +4616,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>215</v>
       </c>
@@ -4629,7 +4631,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>215</v>
       </c>
@@ -4644,7 +4646,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
@@ -4659,7 +4661,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>215</v>
       </c>
@@ -4674,7 +4676,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>215</v>
       </c>
@@ -4689,7 +4691,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>215</v>
       </c>
@@ -4704,7 +4706,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>215</v>
       </c>
@@ -4719,7 +4721,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>215</v>
       </c>
@@ -4734,7 +4736,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>215</v>
       </c>
@@ -4749,7 +4751,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>215</v>
       </c>
@@ -4764,7 +4766,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>215</v>
       </c>
@@ -4779,7 +4781,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>215</v>
       </c>
@@ -4794,7 +4796,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>215</v>
       </c>
@@ -4809,7 +4811,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>215</v>
       </c>
@@ -4824,7 +4826,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>215</v>
       </c>
@@ -4839,7 +4841,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>215</v>
       </c>
@@ -4874,18 +4876,18 @@
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.07421875" customWidth="1"/>
+    <col min="9" max="9" width="12.109375" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.84375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.53515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>170</v>
       </c>
@@ -4935,7 +4937,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U2" t="s">
         <v>183</v>
       </c>
@@ -4943,7 +4945,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U3" t="s">
         <v>184</v>
       </c>
@@ -4951,7 +4953,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U4" t="s">
         <v>186</v>
       </c>
@@ -4959,7 +4961,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U5" t="s">
         <v>187</v>
       </c>
@@ -4967,7 +4969,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U6" t="s">
         <v>189</v>
       </c>
@@ -4975,12 +4977,12 @@
         <v>87</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U7" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="U8" t="s">
         <v>191</v>
       </c>
@@ -5006,20 +5008,20 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.15234375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.3046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.23046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>219</v>
       </c>
@@ -5048,7 +5050,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>217</v>
       </c>
@@ -5080,7 +5082,7 @@
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>217</v>
       </c>
@@ -5112,7 +5114,7 @@
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>217</v>
       </c>
@@ -5144,7 +5146,7 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>217</v>
       </c>
@@ -5176,7 +5178,7 @@
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>217</v>
       </c>
@@ -5203,7 +5205,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>217</v>
       </c>
@@ -5230,7 +5232,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>217</v>
       </c>
@@ -5257,7 +5259,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>217</v>
       </c>
@@ -5284,7 +5286,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>217</v>
       </c>
@@ -5331,21 +5333,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA51A6B7-E36D-420E-A2B8-AD7FB5872218}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.07421875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.23046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.3046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>472</v>
       </c>
@@ -5365,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="17">
         <v>2</v>
       </c>
@@ -5385,7 +5387,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="17">
         <v>0</v>
       </c>
@@ -5405,7 +5407,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="17">
         <v>3</v>
       </c>
@@ -5438,13 +5440,13 @@
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.07421875" customWidth="1"/>
-    <col min="2" max="2" width="8.84375" style="4"/>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>44</v>
       </c>
@@ -5452,7 +5454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>45</v>
       </c>
@@ -5460,7 +5462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>46</v>
       </c>
@@ -5468,7 +5470,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
@@ -5476,7 +5478,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>48</v>
       </c>
@@ -5494,21 +5496,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D077A5-E46E-4ED9-B547-F70AD3D26657}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.07421875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" style="4"/>
-    <col min="4" max="4" width="7.3046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3046875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.53515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="7.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -5528,7 +5530,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
         <v>26</v>
       </c>
@@ -5549,7 +5551,7 @@
         <v>44197</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
         <v>195</v>
       </c>
@@ -5570,7 +5572,7 @@
         <v>44198</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>192</v>
       </c>
@@ -5591,7 +5593,7 @@
         <v>44199</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
         <v>193</v>
       </c>
@@ -5612,7 +5614,7 @@
         <v>44200</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
         <v>194</v>
       </c>
@@ -5633,7 +5635,7 @@
         <v>44201</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
         <v>196</v>
       </c>
@@ -5654,7 +5656,7 @@
         <v>44567</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
         <v>32</v>
       </c>
@@ -5675,7 +5677,7 @@
         <v>44203</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="12" t="s">
         <v>197</v>
       </c>
@@ -5696,7 +5698,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="12" t="s">
         <v>36</v>
       </c>
@@ -5717,7 +5719,7 @@
         <v>44235</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="12" t="s">
         <v>38</v>
       </c>
@@ -5738,7 +5740,7 @@
         <v>44237</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="12" t="s">
         <v>198</v>
       </c>
@@ -5759,7 +5761,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="12" t="s">
         <v>199</v>
       </c>
@@ -5780,7 +5782,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="12" t="s">
         <v>200</v>
       </c>
@@ -5801,7 +5803,7 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="12" t="s">
         <v>201</v>
       </c>
@@ -5822,11 +5824,11 @@
         <v>44242</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
     </row>
@@ -5860,24 +5862,24 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.3046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.69140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.3046875" customWidth="1"/>
-    <col min="7" max="7" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.84375" customWidth="1"/>
-    <col min="9" max="9" width="15.53515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.23046875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.53515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.53515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="9" max="9" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>53</v>
       </c>
@@ -5918,7 +5920,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -5967,7 +5969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>216</v>
       </c>
@@ -6016,7 +6018,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>217</v>
       </c>
@@ -6063,7 +6065,7 @@
       <c r="Q4" s="10"/>
       <c r="R4" s="10"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
       <c r="B5" s="10"/>
       <c r="C5" s="10"/>
@@ -6103,15 +6105,15 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.07421875" customWidth="1"/>
-    <col min="3" max="3" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>72</v>
       </c>
@@ -6125,7 +6127,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -6139,7 +6141,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -6153,7 +6155,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -6167,7 +6169,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -6181,7 +6183,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -6195,7 +6197,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>216</v>
       </c>
@@ -6209,7 +6211,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>216</v>
       </c>
@@ -6223,7 +6225,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>216</v>
       </c>
@@ -6234,7 +6236,7 @@
         <v>44354</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>216</v>
       </c>
@@ -6245,7 +6247,7 @@
         <v>44438</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>216</v>
       </c>
@@ -6256,7 +6258,7 @@
         <v>44627</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>216</v>
       </c>
@@ -6283,24 +6285,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8482F8C3-6DCA-424C-81AE-BDA1451F2AAD}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.53515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.53515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="10.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.07421875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.69140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.84375" style="7"/>
-    <col min="9" max="9" width="9.23046875" style="7"/>
-    <col min="10" max="10" width="14.84375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="7"/>
+    <col min="9" max="9" width="9.21875" style="7"/>
+    <col min="10" max="10" width="14.88671875" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>218</v>
       </c>
@@ -6332,7 +6334,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>195</v>
       </c>
@@ -6365,7 +6367,7 @@
         <v>Tiago Cancado</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>192</v>
       </c>
@@ -6398,7 +6400,7 @@
         <v>Joao Silva</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>193</v>
       </c>
@@ -6431,7 +6433,7 @@
         <v>Manel Costa</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>194</v>
       </c>
@@ -6464,7 +6466,7 @@
         <v>Xico Ferreira</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -6497,7 +6499,7 @@
         <v>Nel Moleiro</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>197</v>
       </c>
@@ -6530,7 +6532,7 @@
         <v>Zé do Bento</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>36</v>
       </c>
@@ -6563,7 +6565,7 @@
         <v>Tó Farrulo</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
@@ -6596,7 +6598,7 @@
         <v>Tino das Cruzes</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="28" t="s">
         <v>195</v>
       </c>
@@ -6629,7 +6631,7 @@
         <v>Tiago Cancado</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
         <v>192</v>
       </c>
@@ -6662,7 +6664,7 @@
         <v>Joao Silva</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="28" t="s">
         <v>193</v>
       </c>
@@ -6695,7 +6697,7 @@
         <v>Manel Costa</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="28" t="s">
         <v>194</v>
       </c>
@@ -6728,7 +6730,7 @@
         <v>Xico Ferreira</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="28" t="s">
         <v>32</v>
       </c>
@@ -6761,7 +6763,7 @@
         <v>Nel Moleiro</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="28" t="s">
         <v>197</v>
       </c>
@@ -6794,7 +6796,7 @@
         <v>Zé do Bento</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="28" t="s">
         <v>36</v>
       </c>
@@ -6827,7 +6829,7 @@
         <v>Tó Farrulo</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="28" t="s">
         <v>38</v>
       </c>
@@ -6875,14 +6877,14 @@
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
         <v>227</v>
       </c>
@@ -6893,7 +6895,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -6905,7 +6907,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -6917,7 +6919,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -6929,7 +6931,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -6941,7 +6943,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -6953,7 +6955,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -6965,7 +6967,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -6977,7 +6979,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -6989,7 +6991,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>216</v>
       </c>
@@ -7001,7 +7003,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>216</v>
       </c>
@@ -7013,7 +7015,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>216</v>
       </c>
@@ -7025,7 +7027,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>216</v>
       </c>
@@ -7037,7 +7039,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>216</v>
       </c>
@@ -7049,7 +7051,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>216</v>
       </c>
@@ -7061,7 +7063,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>216</v>
       </c>
@@ -7073,7 +7075,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>216</v>
       </c>
@@ -7085,7 +7087,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>216</v>
       </c>
@@ -7097,7 +7099,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>216</v>
       </c>
@@ -7109,7 +7111,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>216</v>
       </c>
@@ -7121,7 +7123,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>216</v>
       </c>
@@ -7133,7 +7135,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>217</v>
       </c>
@@ -7144,7 +7146,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>217</v>
       </c>
@@ -7155,7 +7157,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>217</v>
       </c>
@@ -7166,7 +7168,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>217</v>
       </c>
@@ -7177,7 +7179,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>217</v>
       </c>
@@ -7188,7 +7190,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>217</v>
       </c>
@@ -7199,7 +7201,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>217</v>
       </c>
@@ -7210,7 +7212,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>217</v>
       </c>
@@ -7221,7 +7223,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>217</v>
       </c>
@@ -7232,7 +7234,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>217</v>
       </c>
@@ -7243,7 +7245,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>217</v>
       </c>
@@ -7254,7 +7256,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>217</v>
       </c>
@@ -7265,7 +7267,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>217</v>
       </c>
@@ -7276,7 +7278,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>217</v>
       </c>
@@ -7287,7 +7289,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>217</v>
       </c>
@@ -7312,13 +7314,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C1" s="1" t="s">
         <v>203</v>
       </c>
@@ -7341,7 +7343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.4">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.3">
       <c r="C2" s="10" t="s">
         <v>11</v>
       </c>
@@ -7378,19 +7380,19 @@
       <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.84375" style="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.84375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.84375" style="17"/>
-    <col min="4" max="4" width="15.84375" style="10" customWidth="1"/>
-    <col min="5" max="5" width="12.3046875" style="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.07421875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="27.53515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="17"/>
+    <col min="4" max="4" width="15.88671875" style="10" customWidth="1"/>
+    <col min="5" max="5" width="12.33203125" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" style="10" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="10" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="23" t="s">
         <v>227</v>
       </c>
@@ -7422,7 +7424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>215</v>
       </c>
@@ -7454,7 +7456,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="10" t="s">
         <v>215</v>
       </c>
@@ -7482,7 +7484,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>215</v>
       </c>
@@ -7510,7 +7512,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>215</v>
       </c>
@@ -7535,7 +7537,7 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>215</v>
       </c>
@@ -7560,7 +7562,7 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>215</v>
       </c>
@@ -7585,7 +7587,7 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>215</v>
       </c>
@@ -7612,7 +7614,7 @@
       </c>
       <c r="I8" s="25"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="10" t="s">
         <v>215</v>
       </c>
@@ -7637,7 +7639,7 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="10" t="s">
         <v>215</v>
       </c>
@@ -7662,7 +7664,7 @@
       <c r="H10" s="13"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="10" t="s">
         <v>215</v>
       </c>
@@ -7687,7 +7689,7 @@
       <c r="H11" s="13"/>
       <c r="I11" s="13"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>215</v>
       </c>
@@ -7712,7 +7714,7 @@
       <c r="H12" s="13"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="10" t="s">
         <v>215</v>
       </c>
@@ -7737,7 +7739,7 @@
       <c r="H13" s="13"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="10" t="s">
         <v>215</v>
       </c>
@@ -7762,7 +7764,7 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="10" t="s">
         <v>215</v>
       </c>
@@ -7787,7 +7789,7 @@
       <c r="H15" s="13"/>
       <c r="I15" s="13"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>215</v>
       </c>
@@ -7812,7 +7814,7 @@
       <c r="H16" s="13"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
         <v>215</v>
       </c>
@@ -7837,7 +7839,7 @@
       <c r="H17" s="13"/>
       <c r="I17" s="13"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>215</v>
       </c>
@@ -7862,7 +7864,7 @@
       <c r="H18" s="13"/>
       <c r="I18" s="13"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>215</v>
       </c>
@@ -7887,7 +7889,7 @@
       <c r="H19" s="13"/>
       <c r="I19" s="13"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>215</v>
       </c>
@@ -7912,7 +7914,7 @@
       <c r="H20" s="13"/>
       <c r="I20" s="13"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>215</v>
       </c>
@@ -7937,7 +7939,7 @@
       <c r="H21" s="13"/>
       <c r="I21" s="13"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>215</v>
       </c>
@@ -7962,7 +7964,7 @@
       <c r="H22" s="13"/>
       <c r="I22" s="13"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>215</v>
       </c>
@@ -7987,7 +7989,7 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>215</v>
       </c>
@@ -8012,7 +8014,7 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>215</v>
       </c>
@@ -8037,7 +8039,7 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>215</v>
       </c>
@@ -8062,7 +8064,7 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>215</v>
       </c>
@@ -8087,7 +8089,7 @@
       <c r="H27" s="13"/>
       <c r="I27" s="13"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>215</v>
       </c>
@@ -8112,7 +8114,7 @@
       <c r="H28" s="13"/>
       <c r="I28" s="13"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>215</v>
       </c>
@@ -8137,7 +8139,7 @@
       <c r="H29" s="13"/>
       <c r="I29" s="13"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>215</v>
       </c>
@@ -8162,7 +8164,7 @@
       <c r="H30" s="13"/>
       <c r="I30" s="13"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>215</v>
       </c>
@@ -8187,7 +8189,7 @@
       <c r="H31" s="13"/>
       <c r="I31" s="13"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>216</v>
       </c>
@@ -8212,7 +8214,7 @@
       <c r="H32" s="13"/>
       <c r="I32" s="13"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>216</v>
       </c>
@@ -8237,7 +8239,7 @@
       <c r="H33" s="13"/>
       <c r="I33" s="13"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>216</v>
       </c>
@@ -8262,7 +8264,7 @@
       <c r="H34" s="13"/>
       <c r="I34" s="13"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>216</v>
       </c>
@@ -8291,7 +8293,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>216</v>
       </c>
@@ -8320,7 +8322,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>216</v>
       </c>
@@ -8349,7 +8351,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="10" t="s">
         <v>216</v>
       </c>
@@ -8378,7 +8380,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="10" t="s">
         <v>216</v>
       </c>
@@ -8407,7 +8409,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="10" t="s">
         <v>216</v>
       </c>
@@ -8436,7 +8438,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>216</v>
       </c>
@@ -8465,7 +8467,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>216</v>
       </c>
@@ -8490,7 +8492,7 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="10" t="s">
         <v>216</v>
       </c>
@@ -8515,7 +8517,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="13"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="10" t="s">
         <v>216</v>
       </c>
@@ -8540,7 +8542,7 @@
       <c r="H44" s="13"/>
       <c r="I44" s="13"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>216</v>
       </c>
@@ -8565,7 +8567,7 @@
       <c r="H45" s="13"/>
       <c r="I45" s="13"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="10" t="s">
         <v>216</v>
       </c>
@@ -8590,7 +8592,7 @@
       <c r="H46" s="13"/>
       <c r="I46" s="13"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="10" t="s">
         <v>216</v>
       </c>
@@ -8615,7 +8617,7 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="10" t="s">
         <v>216</v>
       </c>
@@ -8640,7 +8642,7 @@
       <c r="H48" s="13"/>
       <c r="I48" s="13"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="10" t="s">
         <v>216</v>
       </c>
@@ -8665,7 +8667,7 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>216</v>
       </c>
@@ -8690,7 +8692,7 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>216</v>
       </c>
@@ -8715,7 +8717,7 @@
       <c r="H51" s="13"/>
       <c r="I51" s="13"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>216</v>
       </c>
@@ -8740,7 +8742,7 @@
       <c r="H52" s="13"/>
       <c r="I52" s="13"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>216</v>
       </c>
@@ -8765,7 +8767,7 @@
       <c r="H53" s="13"/>
       <c r="I53" s="13"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>216</v>
       </c>
@@ -8790,7 +8792,7 @@
       <c r="H54" s="13"/>
       <c r="I54" s="13"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>216</v>
       </c>
@@ -8815,7 +8817,7 @@
       <c r="H55" s="13"/>
       <c r="I55" s="13"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="10" t="s">
         <v>216</v>
       </c>
@@ -8840,7 +8842,7 @@
       <c r="H56" s="13"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="10" t="s">
         <v>216</v>
       </c>
@@ -8865,7 +8867,7 @@
       <c r="H57" s="13"/>
       <c r="I57" s="13"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="10" t="s">
         <v>216</v>
       </c>
@@ -8890,7 +8892,7 @@
       <c r="H58" s="13"/>
       <c r="I58" s="13"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
         <v>216</v>
       </c>
@@ -8915,7 +8917,7 @@
       <c r="H59" s="13"/>
       <c r="I59" s="13"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="10" t="s">
         <v>216</v>
       </c>
@@ -8940,7 +8942,7 @@
       <c r="H60" s="13"/>
       <c r="I60" s="13"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>216</v>
       </c>
@@ -8965,7 +8967,7 @@
       <c r="H61" s="13"/>
       <c r="I61" s="13"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>216</v>
       </c>
@@ -8990,7 +8992,7 @@
       <c r="H62" s="13"/>
       <c r="I62" s="13"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>216</v>
       </c>
@@ -9015,7 +9017,7 @@
       <c r="H63" s="13"/>
       <c r="I63" s="13"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
         <v>216</v>
       </c>
@@ -9040,7 +9042,7 @@
       <c r="H64" s="13"/>
       <c r="I64" s="13"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="10" t="s">
         <v>216</v>
       </c>
@@ -9065,7 +9067,7 @@
       <c r="H65" s="13"/>
       <c r="I65" s="13"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="10" t="s">
         <v>216</v>
       </c>
@@ -9090,7 +9092,7 @@
       <c r="H66" s="13"/>
       <c r="I66" s="13"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="10" t="s">
         <v>216</v>
       </c>
@@ -9119,7 +9121,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="10" t="s">
         <v>217</v>
       </c>
@@ -9144,7 +9146,7 @@
       <c r="H68" s="13"/>
       <c r="I68" s="13"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>217</v>
       </c>
@@ -9171,7 +9173,7 @@
       </c>
       <c r="I69" s="13"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="10" t="s">
         <v>217</v>
       </c>
@@ -9209,12 +9211,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9421,15 +9420,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9454,10 +9457,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Refactoring: ResourceService: update projectRole (addresses #275)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/91e2d21952d024e0/Documentos/Switch/projectg2/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{ADFCC498-6C4D-445F-BABD-7A26CACB6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{162A7242-D61A-409F-9361-2B9D8A5114E7}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{ADFCC498-6C4D-445F-BABD-7A26CACB6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{537645FE-C42D-4B2C-8917-07A38BF753C3}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" tabRatio="938" firstSheet="2" activeTab="5" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" tabRatio="938" activeTab="5" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -2120,8 +2120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AF82CFE-028A-48A4-A712-2087D6C160AE}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6285,8 +6285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8482F8C3-6DCA-424C-81AE-BDA1451F2AAD}">
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6434,7 +6434,7 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="11" t="s">
         <v>194</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -6731,7 +6731,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="11" t="s">
         <v>32</v>
       </c>
       <c r="B14" s="28" t="s">
@@ -6864,8 +6864,12 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A5" r:id="rId1" xr:uid="{9DE76BD9-6A8C-413F-9F64-B0EE7DFE3DD5}"/>
+    <hyperlink ref="A14" r:id="rId2" xr:uid="{454CFFB5-B1D5-4196-BCA2-E0C5C35215BF}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Refactoring: ResourceController: Integration tests (addresses #275)
</commit_message>
<xml_diff>
--- a/src/main/resources/data.xlsx
+++ b/src/main/resources/data.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{ADFCC498-6C4D-445F-BABD-7A26CACB6376}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="48" xr10:uidLastSave="{537645FE-C42D-4B2C-8917-07A38BF753C3}"/>
   <bookViews>
-    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8964" tabRatio="938" activeTab="5" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="8964" tabRatio="938" activeTab="5" xr2:uid="{17341BA7-7E24-41D8-A92D-79256BC3D291}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -9215,9 +9215,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9424,19 +9427,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9461,9 +9460,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{552A2396-49F4-45F5-9D44-9C3125763CF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{41EAF4CE-5C55-41AC-946B-5BEC082284DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>